<commit_message>
added root hair consumption
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_09_22.xlsx
+++ b/simulations/inputs/Scenarios_24_09_22.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6942D5-0CD0-488D-8DC4-61173F9003DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F483309-5B58-4B1F-AD30-3D0C21747D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2866" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="620">
   <si>
     <t>input_file</t>
   </si>
@@ -1506,9 +1506,6 @@
     <t>NW_collar_Fischer_1966_Reicoski_1994.csv</t>
   </si>
   <si>
-    <t>C_mineralN_soil</t>
-  </si>
-  <si>
     <t>mol.m-3</t>
   </si>
   <si>
@@ -1557,9 +1554,6 @@
     <t>adim</t>
   </si>
   <si>
-    <t>C_mineralN_patch</t>
-  </si>
-  <si>
     <t>patch_depth_mineralN</t>
   </si>
   <si>
@@ -1870,6 +1864,36 @@
   </si>
   <si>
     <t>Input_RSML_R4_D01</t>
+  </si>
+  <si>
+    <t>content_mineralN_soil</t>
+  </si>
+  <si>
+    <t>content_mineralN_patch</t>
+  </si>
+  <si>
+    <t>water_moisture_patch</t>
+  </si>
+  <si>
+    <t>patch_depth_water_moisture</t>
+  </si>
+  <si>
+    <t>patch_uniform_width_water_moisture</t>
+  </si>
+  <si>
+    <t>patch_transition_water_moisture</t>
+  </si>
+  <si>
+    <t>water moisture in a located patch in soil</t>
+  </si>
+  <si>
+    <t>Depth of a water moisture patch in soil</t>
+  </si>
+  <si>
+    <t>Width of the zone of the patch with uniform water moisture</t>
+  </si>
+  <si>
+    <t>Variance of the normal law smooting the boundary transition of a moisture patch with the background concentration</t>
   </si>
 </sst>
 </file>
@@ -3062,13 +3086,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AO225"/>
+  <dimension ref="A1:AO229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="AA181" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H191" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AD227" sqref="AD227"/>
+      <selection pane="bottomRight" activeCell="L237" sqref="L237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3106,223 +3130,223 @@
         <v>378</v>
       </c>
       <c r="H1" s="36" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="I1" s="36"/>
       <c r="J1" s="36" t="s">
+        <v>576</v>
+      </c>
+      <c r="K1" s="36" t="s">
+        <v>577</v>
+      </c>
+      <c r="L1" s="36" t="s">
         <v>578</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="M1" s="36" t="s">
         <v>579</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="N1" s="36" t="s">
         <v>580</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="O1" s="36" t="s">
         <v>581</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>582</v>
       </c>
-      <c r="O1" s="36" t="s">
-        <v>583</v>
-      </c>
-      <c r="P1" s="36" t="s">
-        <v>584</v>
-      </c>
       <c r="Q1" s="36" t="s">
+        <v>588</v>
+      </c>
+      <c r="R1" s="36" t="s">
+        <v>589</v>
+      </c>
+      <c r="S1" s="36" t="s">
         <v>590</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="T1" s="36" t="s">
         <v>591</v>
       </c>
-      <c r="S1" s="36" t="s">
-        <v>592</v>
-      </c>
-      <c r="T1" s="36" t="s">
-        <v>593</v>
-      </c>
       <c r="U1" s="36" t="s">
+        <v>596</v>
+      </c>
+      <c r="V1" s="36" t="s">
+        <v>597</v>
+      </c>
+      <c r="W1" s="36" t="s">
         <v>598</v>
       </c>
-      <c r="V1" s="36" t="s">
-        <v>599</v>
-      </c>
-      <c r="W1" s="36" t="s">
-        <v>600</v>
-      </c>
       <c r="X1" s="36" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="Y1" s="36" t="s">
+        <v>605</v>
+      </c>
+      <c r="Z1" s="36" t="s">
+        <v>606</v>
+      </c>
+      <c r="AA1" s="36" t="s">
         <v>607</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="AB1" s="36" t="s">
         <v>608</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AC1" s="36" t="s">
         <v>609</v>
-      </c>
-      <c r="AB1" s="36" t="s">
-        <v>610</v>
-      </c>
-      <c r="AC1" s="36" t="s">
-        <v>611</v>
       </c>
       <c r="AD1" s="36"/>
       <c r="AE1" s="36" t="s">
+        <v>533</v>
+      </c>
+      <c r="AF1" s="36" t="s">
         <v>535</v>
       </c>
-      <c r="AF1" s="36" t="s">
-        <v>537</v>
-      </c>
       <c r="AG1" s="36" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="AH1" s="36" t="s">
+        <v>539</v>
+      </c>
+      <c r="AI1" s="36" t="s">
         <v>541</v>
       </c>
-      <c r="AI1" s="36" t="s">
-        <v>543</v>
-      </c>
       <c r="AJ1" s="36" t="s">
+        <v>546</v>
+      </c>
+      <c r="AK1" s="36" t="s">
+        <v>550</v>
+      </c>
+      <c r="AL1" s="36" t="s">
         <v>548</v>
       </c>
-      <c r="AK1" s="36" t="s">
-        <v>552</v>
-      </c>
-      <c r="AL1" s="36" t="s">
-        <v>550</v>
-      </c>
       <c r="AM1" s="36" t="s">
+        <v>560</v>
+      </c>
+      <c r="AN1" s="36" t="s">
         <v>562</v>
       </c>
-      <c r="AN1" s="36" t="s">
-        <v>564</v>
-      </c>
       <c r="AO1" s="36" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
+        <v>527</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E2" s="75" t="s">
         <v>529</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>530</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>528</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>577</v>
-      </c>
-      <c r="E2" s="75" t="s">
-        <v>531</v>
       </c>
       <c r="F2" s="75" t="s">
         <v>91</v>
       </c>
       <c r="G2" s="76" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="H2" s="100" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="I2" s="100"/>
       <c r="J2" s="100" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
       <c r="K2" s="100" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
       <c r="L2" s="100" t="s">
+        <v>532</v>
+      </c>
+      <c r="M2" s="100" t="s">
+        <v>583</v>
+      </c>
+      <c r="N2" s="100" t="s">
+        <v>584</v>
+      </c>
+      <c r="O2" s="100" t="s">
+        <v>585</v>
+      </c>
+      <c r="P2" s="100" t="s">
+        <v>536</v>
+      </c>
+      <c r="Q2" s="100" t="s">
+        <v>592</v>
+      </c>
+      <c r="R2" s="100" t="s">
+        <v>593</v>
+      </c>
+      <c r="S2" s="100" t="s">
+        <v>594</v>
+      </c>
+      <c r="T2" s="100" t="s">
+        <v>537</v>
+      </c>
+      <c r="U2" s="100" t="s">
+        <v>599</v>
+      </c>
+      <c r="V2" s="100" t="s">
+        <v>600</v>
+      </c>
+      <c r="W2" s="100" t="s">
+        <v>601</v>
+      </c>
+      <c r="X2" s="100" t="s">
+        <v>602</v>
+      </c>
+      <c r="Y2" s="100" t="s">
+        <v>603</v>
+      </c>
+      <c r="Z2" s="100" t="s">
+        <v>604</v>
+      </c>
+      <c r="AA2" s="100" t="s">
+        <v>540</v>
+      </c>
+      <c r="AB2" s="100" t="s">
+        <v>542</v>
+      </c>
+      <c r="AC2" s="100" t="s">
         <v>534</v>
-      </c>
-      <c r="M2" s="100" t="s">
-        <v>585</v>
-      </c>
-      <c r="N2" s="100" t="s">
-        <v>586</v>
-      </c>
-      <c r="O2" s="100" t="s">
-        <v>587</v>
-      </c>
-      <c r="P2" s="100" t="s">
-        <v>538</v>
-      </c>
-      <c r="Q2" s="100" t="s">
-        <v>594</v>
-      </c>
-      <c r="R2" s="100" t="s">
-        <v>595</v>
-      </c>
-      <c r="S2" s="100" t="s">
-        <v>596</v>
-      </c>
-      <c r="T2" s="100" t="s">
-        <v>539</v>
-      </c>
-      <c r="U2" s="100" t="s">
-        <v>601</v>
-      </c>
-      <c r="V2" s="100" t="s">
-        <v>602</v>
-      </c>
-      <c r="W2" s="100" t="s">
-        <v>603</v>
-      </c>
-      <c r="X2" s="100" t="s">
-        <v>604</v>
-      </c>
-      <c r="Y2" s="100" t="s">
-        <v>605</v>
-      </c>
-      <c r="Z2" s="100" t="s">
-        <v>606</v>
-      </c>
-      <c r="AA2" s="100" t="s">
-        <v>542</v>
-      </c>
-      <c r="AB2" s="100" t="s">
-        <v>544</v>
-      </c>
-      <c r="AC2" s="100" t="s">
-        <v>536</v>
       </c>
       <c r="AD2" s="100"/>
       <c r="AE2" s="100" t="s">
+        <v>534</v>
+      </c>
+      <c r="AF2" s="100" t="s">
         <v>536</v>
       </c>
-      <c r="AF2" s="100" t="s">
-        <v>538</v>
-      </c>
       <c r="AG2" s="100" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="AH2" s="100" t="s">
+        <v>540</v>
+      </c>
+      <c r="AI2" s="100" t="s">
         <v>542</v>
       </c>
-      <c r="AI2" s="100" t="s">
-        <v>544</v>
-      </c>
       <c r="AJ2" s="100" t="s">
+        <v>547</v>
+      </c>
+      <c r="AK2" s="100" t="s">
         <v>549</v>
       </c>
-      <c r="AK2" s="100" t="s">
+      <c r="AL2" s="100" t="s">
         <v>551</v>
       </c>
-      <c r="AL2" s="100" t="s">
-        <v>553</v>
-      </c>
       <c r="AM2" s="100" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="AN2" s="100" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
       <c r="AO2" s="100" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="3" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3333,10 +3357,10 @@
         <v>471</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>472</v>
@@ -3454,10 +3478,10 @@
         <v>471</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>476</v>
@@ -3575,10 +3599,10 @@
         <v>471</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>486</v>
@@ -3696,10 +3720,10 @@
         <v>471</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>477</v>
@@ -3811,22 +3835,22 @@
     </row>
     <row r="7" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>470</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="G7" s="51">
         <v>0</v>
@@ -3969,10 +3993,10 @@
         <v>470</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>129</v>
@@ -4090,10 +4114,10 @@
         <v>470</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>130</v>
@@ -4211,10 +4235,10 @@
         <v>470</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E10" s="75" t="s">
         <v>444</v>
@@ -4332,10 +4356,10 @@
         <v>470</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>114</v>
@@ -4453,10 +4477,10 @@
         <v>470</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>115</v>
@@ -4574,10 +4598,10 @@
         <v>470</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>123</v>
@@ -4695,10 +4719,10 @@
         <v>470</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>113</v>
@@ -4816,10 +4840,10 @@
         <v>470</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>448</v>
@@ -4937,10 +4961,10 @@
         <v>470</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>131</v>
@@ -5058,10 +5082,10 @@
         <v>470</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>116</v>
@@ -5179,10 +5203,10 @@
         <v>470</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>117</v>
@@ -5300,10 +5324,10 @@
         <v>470</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>455</v>
@@ -5421,10 +5445,10 @@
         <v>470</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>462</v>
@@ -5542,10 +5566,10 @@
         <v>470</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>465</v>
@@ -5663,10 +5687,10 @@
         <v>470</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>467</v>
@@ -5784,10 +5808,10 @@
         <v>470</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>133</v>
@@ -5905,10 +5929,10 @@
         <v>470</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>118</v>
@@ -6026,10 +6050,10 @@
         <v>470</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>363</v>
@@ -6147,10 +6171,10 @@
         <v>470</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>365</v>
@@ -6268,10 +6292,10 @@
         <v>470</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>377</v>
@@ -6389,10 +6413,10 @@
         <v>470</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>373</v>
@@ -6510,10 +6534,10 @@
         <v>470</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>372</v>
@@ -6631,10 +6655,10 @@
         <v>470</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>139</v>
@@ -6752,10 +6776,10 @@
         <v>470</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>119</v>
@@ -6873,10 +6897,10 @@
         <v>470</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>134</v>
@@ -6994,10 +7018,10 @@
         <v>470</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>132</v>
@@ -7115,10 +7139,10 @@
         <v>470</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>454</v>
@@ -7236,10 +7260,10 @@
         <v>470</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>137</v>
@@ -7357,10 +7381,10 @@
         <v>470</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>124</v>
@@ -7478,10 +7502,10 @@
         <v>470</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>125</v>
@@ -7599,10 +7623,10 @@
         <v>470</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>126</v>
@@ -7720,10 +7744,10 @@
         <v>470</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>138</v>
@@ -7841,10 +7865,10 @@
         <v>470</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>127</v>
@@ -7962,10 +7986,10 @@
         <v>470</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>128</v>
@@ -8083,10 +8107,10 @@
         <v>470</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>140</v>
@@ -8204,10 +8228,10 @@
         <v>470</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>141</v>
@@ -8325,10 +8349,10 @@
         <v>470</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>142</v>
@@ -8446,10 +8470,10 @@
         <v>470</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>143</v>
@@ -8567,10 +8591,10 @@
         <v>470</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>144</v>
@@ -8688,10 +8712,10 @@
         <v>470</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>145</v>
@@ -8809,10 +8833,10 @@
         <v>470</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>146</v>
@@ -8930,10 +8954,10 @@
         <v>470</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>147</v>
@@ -9051,10 +9075,10 @@
         <v>470</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>435</v>
@@ -9172,10 +9196,10 @@
         <v>470</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>436</v>
@@ -9293,10 +9317,10 @@
         <v>470</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>457</v>
@@ -9414,10 +9438,10 @@
         <v>470</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>135</v>
@@ -9535,10 +9559,10 @@
         <v>470</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>136</v>
@@ -9656,10 +9680,10 @@
         <v>470</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>120</v>
@@ -9777,10 +9801,10 @@
         <v>470</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>121</v>
@@ -9898,10 +9922,10 @@
         <v>470</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E57" s="12" t="s">
         <v>122</v>
@@ -10019,10 +10043,10 @@
         <v>470</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>148</v>
@@ -10140,10 +10164,10 @@
         <v>470</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>380</v>
@@ -10261,10 +10285,10 @@
         <v>470</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>149</v>
@@ -10382,10 +10406,10 @@
         <v>470</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>150</v>
@@ -10503,10 +10527,10 @@
         <v>470</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>151</v>
@@ -10624,10 +10648,10 @@
         <v>470</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>152</v>
@@ -10745,10 +10769,10 @@
         <v>470</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E64" s="18" t="s">
         <v>284</v>
@@ -10866,10 +10890,10 @@
         <v>470</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E65" s="18" t="s">
         <v>155</v>
@@ -10987,10 +11011,10 @@
         <v>470</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E66" s="18" t="s">
         <v>406</v>
@@ -11108,10 +11132,10 @@
         <v>470</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E67" s="18" t="s">
         <v>153</v>
@@ -11229,10 +11253,10 @@
         <v>470</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>408</v>
@@ -11350,10 +11374,10 @@
         <v>470</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E69" s="18" t="s">
         <v>154</v>
@@ -11471,10 +11495,10 @@
         <v>470</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E70" s="18" t="s">
         <v>288</v>
@@ -11592,10 +11616,10 @@
         <v>470</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>381</v>
@@ -11713,10 +11737,10 @@
         <v>470</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E72" s="18" t="s">
         <v>156</v>
@@ -11834,10 +11858,10 @@
         <v>470</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E73" s="18" t="s">
         <v>157</v>
@@ -11955,10 +11979,10 @@
         <v>470</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E74" s="18" t="s">
         <v>158</v>
@@ -12076,10 +12100,10 @@
         <v>470</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>159</v>
@@ -12197,10 +12221,10 @@
         <v>470</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E76" s="18" t="s">
         <v>160</v>
@@ -12318,10 +12342,10 @@
         <v>470</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E77" s="18" t="s">
         <v>161</v>
@@ -12439,10 +12463,10 @@
         <v>470</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E78" s="34" t="s">
         <v>418</v>
@@ -12560,10 +12584,10 @@
         <v>470</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E79" s="34" t="s">
         <v>412</v>
@@ -12681,10 +12705,10 @@
         <v>470</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E80" s="34" t="s">
         <v>419</v>
@@ -12802,10 +12826,10 @@
         <v>470</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E81" s="34" t="s">
         <v>402</v>
@@ -12923,10 +12947,10 @@
         <v>470</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E82" s="34" t="s">
         <v>415</v>
@@ -13044,10 +13068,10 @@
         <v>470</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E83" s="34" t="s">
         <v>414</v>
@@ -13165,10 +13189,10 @@
         <v>470</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E84" s="34" t="s">
         <v>416</v>
@@ -13286,10 +13310,10 @@
         <v>470</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E85" s="34" t="s">
         <v>403</v>
@@ -13407,10 +13431,10 @@
         <v>470</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E86" s="34" t="s">
         <v>404</v>
@@ -13528,10 +13552,10 @@
         <v>470</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E87" s="18" t="s">
         <v>162</v>
@@ -13649,10 +13673,10 @@
         <v>470</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E88" s="18" t="s">
         <v>163</v>
@@ -13770,10 +13794,10 @@
         <v>470</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E89" s="18" t="s">
         <v>164</v>
@@ -13891,10 +13915,10 @@
         <v>470</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E90" s="18" t="s">
         <v>165</v>
@@ -14012,10 +14036,10 @@
         <v>470</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E91" s="18" t="s">
         <v>166</v>
@@ -14133,10 +14157,10 @@
         <v>470</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E92" s="20" t="s">
         <v>290</v>
@@ -14254,10 +14278,10 @@
         <v>470</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>291</v>
@@ -14375,10 +14399,10 @@
         <v>470</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E94" s="20" t="s">
         <v>295</v>
@@ -14496,10 +14520,10 @@
         <v>470</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E95" s="20" t="s">
         <v>292</v>
@@ -14617,10 +14641,10 @@
         <v>470</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E96" s="20" t="s">
         <v>293</v>
@@ -14738,10 +14762,10 @@
         <v>470</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E97" s="14" t="s">
         <v>171</v>
@@ -14859,10 +14883,10 @@
         <v>470</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E98" s="14" t="s">
         <v>289</v>
@@ -14980,10 +15004,10 @@
         <v>470</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E99" s="14" t="s">
         <v>170</v>
@@ -15101,10 +15125,10 @@
         <v>470</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E100" s="24" t="s">
         <v>176</v>
@@ -15222,10 +15246,10 @@
         <v>470</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E101" s="24" t="s">
         <v>369</v>
@@ -15343,10 +15367,10 @@
         <v>470</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E102" s="24" t="s">
         <v>370</v>
@@ -15464,10 +15488,10 @@
         <v>470</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E103" s="24" t="s">
         <v>371</v>
@@ -15579,16 +15603,16 @@
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E104" s="24" t="s">
         <v>383</v>
@@ -15706,10 +15730,10 @@
         <v>470</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E105" s="24" t="s">
         <v>385</v>
@@ -15821,22 +15845,22 @@
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A106" s="23" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E106" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F106" s="24" t="s">
         <v>505</v>
-      </c>
-      <c r="F106" s="24" t="s">
-        <v>506</v>
       </c>
       <c r="G106" s="58">
         <f t="shared" ref="G106:H106" si="1">G104</f>
@@ -15975,22 +15999,22 @@
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A107" s="23" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E107" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F107" s="24" t="s">
         <v>505</v>
-      </c>
-      <c r="F107" s="24" t="s">
-        <v>506</v>
       </c>
       <c r="G107" s="58">
         <f>3*G104</f>
@@ -16129,22 +16153,22 @@
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A108" s="23" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E108" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F108" s="24" t="s">
         <v>505</v>
-      </c>
-      <c r="F108" s="24" t="s">
-        <v>506</v>
       </c>
       <c r="G108" s="58">
         <f t="shared" ref="G108:H108" si="7">G99</f>
@@ -16283,22 +16307,22 @@
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A109" s="23" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E109" s="24" t="s">
+        <v>504</v>
+      </c>
+      <c r="F109" s="24" t="s">
         <v>505</v>
-      </c>
-      <c r="F109" s="24" t="s">
-        <v>506</v>
       </c>
       <c r="G109" s="58">
         <f>10*G99</f>
@@ -16443,10 +16467,10 @@
         <v>470</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E110" s="24" t="s">
         <v>387</v>
@@ -16564,10 +16588,10 @@
         <v>470</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E111" s="24" t="s">
         <v>389</v>
@@ -16685,10 +16709,10 @@
         <v>470</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E112" s="24" t="s">
         <v>391</v>
@@ -16806,10 +16830,10 @@
         <v>470</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E113" s="24" t="s">
         <v>393</v>
@@ -16927,10 +16951,10 @@
         <v>470</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E114" s="24" t="s">
         <v>421</v>
@@ -17048,10 +17072,10 @@
         <v>470</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E115" s="24" t="s">
         <v>423</v>
@@ -17202,10 +17226,10 @@
         <v>470</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E116" s="24" t="s">
         <v>425</v>
@@ -17350,16 +17374,16 @@
     </row>
     <row r="117" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A117" s="23" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E117" s="24" t="s">
         <v>426</v>
@@ -17471,16 +17495,16 @@
     </row>
     <row r="118" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="23" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E118" s="24" t="s">
         <v>427</v>
@@ -17625,16 +17649,16 @@
     </row>
     <row r="119" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A119" s="23" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E119" s="24" t="s">
         <v>428</v>
@@ -17785,10 +17809,10 @@
         <v>470</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E120" s="24" t="s">
         <v>395</v>
@@ -17906,10 +17930,10 @@
         <v>470</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E121" s="24" t="s">
         <v>397</v>
@@ -18027,10 +18051,10 @@
         <v>470</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E122" s="14" t="s">
         <v>172</v>
@@ -18148,10 +18172,10 @@
         <v>470</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E123" s="14" t="s">
         <v>173</v>
@@ -18301,10 +18325,10 @@
         <v>470</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E124" s="14" t="s">
         <v>174</v>
@@ -18422,10 +18446,10 @@
         <v>470</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E125" s="14" t="s">
         <v>175</v>
@@ -18543,10 +18567,10 @@
         <v>470</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E126" s="14" t="s">
         <v>450</v>
@@ -18664,10 +18688,10 @@
         <v>470</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E127" s="14" t="s">
         <v>452</v>
@@ -18785,10 +18809,10 @@
         <v>470</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E128" s="69" t="s">
         <v>178</v>
@@ -18904,10 +18928,10 @@
         <v>470</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E129" s="69" t="s">
         <v>441</v>
@@ -19023,10 +19047,10 @@
         <v>470</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E130" s="69" t="s">
         <v>446</v>
@@ -19144,10 +19168,10 @@
         <v>470</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E131" s="22" t="s">
         <v>177</v>
@@ -19265,10 +19289,10 @@
         <v>470</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E132" s="22" t="s">
         <v>438</v>
@@ -19386,10 +19410,10 @@
         <v>470</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E133" s="22" t="s">
         <v>311</v>
@@ -19507,10 +19531,10 @@
         <v>470</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E134" s="22" t="s">
         <v>312</v>
@@ -19628,10 +19652,10 @@
         <v>470</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E135" s="22" t="s">
         <v>313</v>
@@ -19749,10 +19773,10 @@
         <v>470</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E136" s="22" t="s">
         <v>314</v>
@@ -19870,10 +19894,10 @@
         <v>470</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E137" s="22" t="s">
         <v>178</v>
@@ -19991,10 +20015,10 @@
         <v>470</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E138" s="22" t="s">
         <v>315</v>
@@ -20112,10 +20136,10 @@
         <v>470</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E139" s="22" t="s">
         <v>316</v>
@@ -20233,10 +20257,10 @@
         <v>470</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E140" s="22" t="s">
         <v>317</v>
@@ -20354,10 +20378,10 @@
         <v>470</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E141" s="22" t="s">
         <v>318</v>
@@ -20475,10 +20499,10 @@
         <v>470</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E142" s="22" t="s">
         <v>180</v>
@@ -20596,10 +20620,10 @@
         <v>470</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E143" s="73" t="s">
         <v>181</v>
@@ -20717,10 +20741,10 @@
         <v>470</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E144" s="24" t="s">
         <v>167</v>
@@ -20838,10 +20862,10 @@
         <v>470</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E145" s="24" t="s">
         <v>168</v>
@@ -20959,10 +20983,10 @@
         <v>470</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E146" s="24" t="s">
         <v>169</v>
@@ -21080,10 +21104,10 @@
         <v>470</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E147" s="24" t="s">
         <v>183</v>
@@ -21201,10 +21225,10 @@
         <v>470</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E148" s="24" t="s">
         <v>303</v>
@@ -21322,10 +21346,10 @@
         <v>470</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E149" s="24" t="s">
         <v>304</v>
@@ -21443,10 +21467,10 @@
         <v>470</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E150" s="24" t="s">
         <v>305</v>
@@ -21564,10 +21588,10 @@
         <v>470</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E151" s="24" t="s">
         <v>306</v>
@@ -21685,10 +21709,10 @@
         <v>470</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E152" s="24" t="s">
         <v>184</v>
@@ -21806,10 +21830,10 @@
         <v>470</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E153" s="14" t="s">
         <v>186</v>
@@ -21927,10 +21951,10 @@
         <v>470</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E154" s="14" t="s">
         <v>307</v>
@@ -22048,10 +22072,10 @@
         <v>470</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E155" s="14" t="s">
         <v>308</v>
@@ -22169,10 +22193,10 @@
         <v>470</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E156" s="14" t="s">
         <v>309</v>
@@ -22290,10 +22314,10 @@
         <v>470</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E157" s="14" t="s">
         <v>310</v>
@@ -22411,10 +22435,10 @@
         <v>470</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E158" s="14" t="s">
         <v>185</v>
@@ -22532,10 +22556,10 @@
         <v>470</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>187</v>
@@ -22653,10 +22677,10 @@
         <v>470</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>298</v>
@@ -22774,10 +22798,10 @@
         <v>470</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E161" s="10" t="s">
         <v>299</v>
@@ -22895,10 +22919,10 @@
         <v>470</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E162" s="10" t="s">
         <v>300</v>
@@ -23016,10 +23040,10 @@
         <v>470</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E163" s="10" t="s">
         <v>302</v>
@@ -23137,10 +23161,10 @@
         <v>470</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E164" s="10" t="s">
         <v>188</v>
@@ -23258,10 +23282,10 @@
         <v>470</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E165" s="26" t="s">
         <v>189</v>
@@ -23379,10 +23403,10 @@
         <v>470</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E166" s="26" t="s">
         <v>319</v>
@@ -23500,10 +23524,10 @@
         <v>470</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E167" s="26" t="s">
         <v>320</v>
@@ -23621,10 +23645,10 @@
         <v>470</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E168" s="26" t="s">
         <v>321</v>
@@ -23742,10 +23766,10 @@
         <v>470</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E169" s="26" t="s">
         <v>322</v>
@@ -23863,10 +23887,10 @@
         <v>470</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E170" s="26" t="s">
         <v>190</v>
@@ -23984,10 +24008,10 @@
         <v>470</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E171" s="32" t="s">
         <v>191</v>
@@ -24105,10 +24129,10 @@
         <v>470</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E172" s="32" t="s">
         <v>323</v>
@@ -24226,10 +24250,10 @@
         <v>470</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E173" s="32" t="s">
         <v>324</v>
@@ -24347,10 +24371,10 @@
         <v>470</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E174" s="32" t="s">
         <v>325</v>
@@ -24468,10 +24492,10 @@
         <v>470</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E175" s="32" t="s">
         <v>326</v>
@@ -24589,10 +24613,10 @@
         <v>470</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E176" s="32" t="s">
         <v>192</v>
@@ -24710,10 +24734,10 @@
         <v>470</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E177" s="12" t="s">
         <v>327</v>
@@ -24831,10 +24855,10 @@
         <v>470</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E178" s="12" t="s">
         <v>329</v>
@@ -24952,10 +24976,10 @@
         <v>470</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E179" s="12" t="s">
         <v>330</v>
@@ -25073,10 +25097,10 @@
         <v>470</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E180" s="12" t="s">
         <v>331</v>
@@ -25194,10 +25218,10 @@
         <v>470</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E181" s="12" t="s">
         <v>332</v>
@@ -25315,10 +25339,10 @@
         <v>470</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E182" s="12" t="s">
         <v>349</v>
@@ -25436,10 +25460,10 @@
         <v>470</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E183" s="12" t="s">
         <v>350</v>
@@ -25557,10 +25581,10 @@
         <v>470</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E184" s="28" t="s">
         <v>351</v>
@@ -25678,10 +25702,10 @@
         <v>470</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E185" s="28" t="s">
         <v>333</v>
@@ -25799,10 +25823,10 @@
         <v>470</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E186" s="28" t="s">
         <v>334</v>
@@ -25920,10 +25944,10 @@
         <v>470</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E187" s="28" t="s">
         <v>335</v>
@@ -26041,10 +26065,10 @@
         <v>470</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E188" s="28" t="s">
         <v>336</v>
@@ -26162,10 +26186,10 @@
         <v>470</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E189" s="28" t="s">
         <v>353</v>
@@ -26283,10 +26307,10 @@
         <v>470</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E190" s="24" t="s">
         <v>193</v>
@@ -26404,10 +26428,10 @@
         <v>470</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E191" s="24" t="s">
         <v>337</v>
@@ -26525,10 +26549,10 @@
         <v>470</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E192" s="24" t="s">
         <v>338</v>
@@ -26646,10 +26670,10 @@
         <v>470</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E193" s="24" t="s">
         <v>339</v>
@@ -26767,10 +26791,10 @@
         <v>470</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E194" s="24" t="s">
         <v>340</v>
@@ -26888,10 +26912,10 @@
         <v>470</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E195" s="24" t="s">
         <v>194</v>
@@ -27009,10 +27033,10 @@
         <v>470</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>355</v>
@@ -27130,10 +27154,10 @@
         <v>470</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>341</v>
@@ -27251,10 +27275,10 @@
         <v>470</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>342</v>
@@ -27372,10 +27396,10 @@
         <v>470</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>343</v>
@@ -27493,10 +27517,10 @@
         <v>470</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>344</v>
@@ -27614,10 +27638,10 @@
         <v>470</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>358</v>
@@ -27735,10 +27759,10 @@
         <v>470</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E202" s="30" t="s">
         <v>356</v>
@@ -27856,10 +27880,10 @@
         <v>470</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E203" s="30" t="s">
         <v>345</v>
@@ -27977,10 +28001,10 @@
         <v>470</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E204" s="30" t="s">
         <v>346</v>
@@ -28098,10 +28122,10 @@
         <v>470</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E205" s="30" t="s">
         <v>347</v>
@@ -28219,10 +28243,10 @@
         <v>470</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E206" s="30" t="s">
         <v>348</v>
@@ -28340,10 +28364,10 @@
         <v>470</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E207" s="30" t="s">
         <v>360</v>
@@ -28461,10 +28485,10 @@
         <v>470</v>
       </c>
       <c r="C208" s="92" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E208" s="93" t="s">
         <v>203</v>
@@ -28576,22 +28600,22 @@
     </row>
     <row r="209" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>490</v>
+        <v>610</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E209" s="30" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F209" s="30" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G209" s="2">
         <v>0.5</v>
@@ -28703,22 +28727,22 @@
     </row>
     <row r="210" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E210" s="30" t="s">
+        <v>494</v>
+      </c>
+      <c r="F210" s="30" t="s">
         <v>495</v>
-      </c>
-      <c r="F210" s="30" t="s">
-        <v>496</v>
       </c>
       <c r="G210" s="97">
         <v>-100000</v>
@@ -28824,22 +28848,22 @@
     </row>
     <row r="211" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>516</v>
+        <v>514</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E211" s="30" t="s">
-        <v>517</v>
+        <v>515</v>
       </c>
       <c r="F211" s="30" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="G211" s="97">
         <v>-100000</v>
@@ -28946,22 +28970,22 @@
     </row>
     <row r="212" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>507</v>
+        <v>611</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E212" s="96" t="s">
-        <v>512</v>
+        <v>510</v>
       </c>
       <c r="F212" s="96" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="G212" s="99">
         <v>0.5</v>
@@ -29067,22 +29091,22 @@
     </row>
     <row r="213" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>508</v>
+        <v>506</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E213" s="96" t="s">
-        <v>513</v>
+        <v>511</v>
       </c>
       <c r="F213" s="96" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="G213" s="99" t="s">
         <v>474</v>
@@ -29188,22 +29212,22 @@
     </row>
     <row r="214" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>509</v>
+        <v>507</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E214" s="96" t="s">
-        <v>514</v>
+        <v>512</v>
       </c>
       <c r="F214" s="96" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="G214" s="99">
         <v>0</v>
@@ -29309,22 +29333,22 @@
     </row>
     <row r="215" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>510</v>
+        <v>508</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E215" s="96" t="s">
-        <v>515</v>
+        <v>513</v>
       </c>
       <c r="F215" s="96" t="s">
-        <v>511</v>
+        <v>509</v>
       </c>
       <c r="G215" s="99">
         <v>1E-3</v>
@@ -29430,22 +29454,22 @@
     </row>
     <row r="216" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>518</v>
+        <v>516</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E216" s="96" t="s">
-        <v>519</v>
+        <v>517</v>
       </c>
       <c r="F216" s="96" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G216" s="99">
         <v>29</v>
@@ -29551,22 +29575,22 @@
     </row>
     <row r="217" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>520</v>
+        <v>518</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E217" s="96" t="s">
-        <v>521</v>
+        <v>519</v>
       </c>
       <c r="F217" s="96" t="s">
-        <v>522</v>
+        <v>520</v>
       </c>
       <c r="G217" s="98">
         <f>1.25*0.000001</f>
@@ -29705,22 +29729,22 @@
     </row>
     <row r="218" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>525</v>
+        <v>523</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E218" s="96" t="s">
-        <v>526</v>
+        <v>524</v>
       </c>
       <c r="F218" s="96" t="s">
-        <v>527</v>
+        <v>525</v>
       </c>
       <c r="G218" s="98">
         <v>2.0000000000000001E-4</v>
@@ -29826,22 +29850,22 @@
     </row>
     <row r="219" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E219" s="96" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
       <c r="F219" s="96" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G219" s="98">
         <v>2.4999999999999998E-12</v>
@@ -29947,22 +29971,22 @@
     </row>
     <row r="220" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E220" s="96" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
       <c r="F220" s="96" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
       <c r="G220" s="98">
         <v>1.2E-8</v>
@@ -30068,22 +30092,22 @@
     </row>
     <row r="221" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E221" s="96" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
       <c r="F221" s="96" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
       <c r="G221" s="98">
         <v>9.9999999999999995E-8</v>
@@ -30189,22 +30213,22 @@
     </row>
     <row r="222" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E222" s="96" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
       <c r="F222" s="96" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="G222" s="98">
         <f>2*0.00001</f>
@@ -30312,22 +30336,22 @@
     </row>
     <row r="223" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>523</v>
+        <v>521</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E223" s="96" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
       <c r="F223" s="96" t="s">
-        <v>524</v>
+        <v>522</v>
       </c>
       <c r="G223" s="98">
         <f>0.00000000000001 * 1000</f>
@@ -30466,22 +30490,22 @@
     </row>
     <row r="224" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E224" s="96" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="F224" s="96" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
       <c r="G224" s="98">
         <f>0.00000000000001 * 10000</f>
@@ -30620,22 +30644,22 @@
     </row>
     <row r="225" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
       <c r="E225" s="96" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
       <c r="F225" s="96" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="G225" s="98">
         <f>0.84*(0.36^2)</f>
@@ -30739,6 +30763,523 @@
       </c>
       <c r="AO225" s="98">
         <v>10</v>
+      </c>
+    </row>
+    <row r="226" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A226" s="2" t="s">
+        <v>612</v>
+      </c>
+      <c r="B226" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C226" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="D226" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E226" s="96" t="s">
+        <v>616</v>
+      </c>
+      <c r="F226" s="96" t="s">
+        <v>490</v>
+      </c>
+      <c r="G226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="H226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="I226" s="99"/>
+      <c r="J226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="K226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="L226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="M226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="N226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="O226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="P226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="Q226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="R226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="S226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="T226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="U226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="V226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="W226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="X226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="Y226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="Z226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AA226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AB226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AC226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AD226" s="99"/>
+      <c r="AE226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AF226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AG226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AH226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AI226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AJ226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AK226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AL226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AM226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AN226" s="99">
+        <v>0.2</v>
+      </c>
+      <c r="AO226" s="99">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A227" s="2" t="s">
+        <v>613</v>
+      </c>
+      <c r="B227" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C227" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="D227" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E227" s="96" t="s">
+        <v>617</v>
+      </c>
+      <c r="F227" s="96" t="s">
+        <v>509</v>
+      </c>
+      <c r="G227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="H227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="I227" s="99"/>
+      <c r="J227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="K227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="L227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="M227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="N227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="O227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="P227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="Q227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="R227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="S227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="T227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="U227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="V227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="W227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="X227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="Y227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="Z227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AA227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AB227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AC227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AD227" s="99"/>
+      <c r="AE227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AF227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AG227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AH227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AI227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AJ227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AK227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AL227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AM227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AN227" s="99" t="s">
+        <v>474</v>
+      </c>
+      <c r="AO227" s="99" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="228" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A228" s="2" t="s">
+        <v>614</v>
+      </c>
+      <c r="B228" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C228" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="D228" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E228" s="96" t="s">
+        <v>618</v>
+      </c>
+      <c r="F228" s="96" t="s">
+        <v>509</v>
+      </c>
+      <c r="G228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="H228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="I228" s="99"/>
+      <c r="J228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="K228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="L228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="M228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="N228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="O228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="P228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="Q228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="R228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="S228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="T228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="U228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="V228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="W228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="X228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="Y228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="Z228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AA228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AB228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AC228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AD228" s="99"/>
+      <c r="AE228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AF228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AG228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AH228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AI228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AJ228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AK228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AL228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AM228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AN228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+      <c r="AO228" s="99">
+        <f>2*0.1</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A229" s="2" t="s">
+        <v>615</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C229" s="2" t="s">
+        <v>526</v>
+      </c>
+      <c r="D229" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="E229" s="96" t="s">
+        <v>619</v>
+      </c>
+      <c r="F229" s="96" t="s">
+        <v>509</v>
+      </c>
+      <c r="G229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="H229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="I229" s="99"/>
+      <c r="J229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="K229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="L229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="M229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="N229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="O229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="P229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="Q229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="R229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="S229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="T229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="U229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="V229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="W229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="X229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="Y229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="Z229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AA229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AB229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AC229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AD229" s="99"/>
+      <c r="AE229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AF229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AG229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AH229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AI229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AK229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AL229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AM229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AN229" s="99">
+        <v>1E-3</v>
+      </c>
+      <c r="AO229" s="99">
+        <v>1E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected soil N content parametrization
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_09_22.xlsx
+++ b/simulations/inputs/Scenarios_24_09_22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F483309-5B58-4B1F-AD30-3D0C21747D97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D980FE-CBD5-4C85-BF26-9ED0F467DA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_as_columns" sheetId="2" r:id="rId1"/>
@@ -1515,9 +1515,6 @@
     <t>Reference_Fischer</t>
   </si>
   <si>
-    <t>water_potential_soil</t>
-  </si>
-  <si>
     <t>Mean soil water potential</t>
   </si>
   <si>
@@ -1894,6 +1891,9 @@
   </si>
   <si>
     <t>Variance of the normal law smooting the boundary transition of a moisture patch with the background concentration</t>
+  </si>
+  <si>
+    <t>soil_moisture</t>
   </si>
 </sst>
 </file>
@@ -3089,10 +3089,10 @@
   <dimension ref="A1:AO229"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H191" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L237" sqref="L237"/>
+      <selection pane="bottomRight" activeCell="K213" sqref="K213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3134,219 +3134,219 @@
       </c>
       <c r="I1" s="36"/>
       <c r="J1" s="36" t="s">
+        <v>575</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>576</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="M1" s="36" t="s">
         <v>578</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="N1" s="36" t="s">
         <v>579</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="O1" s="36" t="s">
         <v>580</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>581</v>
       </c>
-      <c r="P1" s="36" t="s">
-        <v>582</v>
-      </c>
       <c r="Q1" s="36" t="s">
+        <v>587</v>
+      </c>
+      <c r="R1" s="36" t="s">
         <v>588</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="S1" s="36" t="s">
         <v>589</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="T1" s="36" t="s">
         <v>590</v>
       </c>
-      <c r="T1" s="36" t="s">
-        <v>591</v>
-      </c>
       <c r="U1" s="36" t="s">
+        <v>595</v>
+      </c>
+      <c r="V1" s="36" t="s">
         <v>596</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="W1" s="36" t="s">
         <v>597</v>
       </c>
-      <c r="W1" s="36" t="s">
-        <v>598</v>
-      </c>
       <c r="X1" s="36" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
       <c r="Y1" s="36" t="s">
+        <v>604</v>
+      </c>
+      <c r="Z1" s="36" t="s">
         <v>605</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="AA1" s="36" t="s">
         <v>606</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AB1" s="36" t="s">
         <v>607</v>
       </c>
-      <c r="AB1" s="36" t="s">
+      <c r="AC1" s="36" t="s">
         <v>608</v>
-      </c>
-      <c r="AC1" s="36" t="s">
-        <v>609</v>
       </c>
       <c r="AD1" s="36"/>
       <c r="AE1" s="36" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
       <c r="AF1" s="36" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
       <c r="AG1" s="36" t="s">
+        <v>537</v>
+      </c>
+      <c r="AH1" s="36" t="s">
         <v>538</v>
       </c>
-      <c r="AH1" s="36" t="s">
-        <v>539</v>
-      </c>
       <c r="AI1" s="36" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
       <c r="AJ1" s="36" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AK1" s="36" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AL1" s="36" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AM1" s="36" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AN1" s="36" t="s">
+        <v>561</v>
+      </c>
+      <c r="AO1" s="36" t="s">
         <v>562</v>
-      </c>
-      <c r="AO1" s="36" t="s">
-        <v>563</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="74" t="s">
+        <v>526</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>527</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
+        <v>525</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="E2" s="75" t="s">
         <v>528</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>526</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>575</v>
-      </c>
-      <c r="E2" s="75" t="s">
-        <v>529</v>
       </c>
       <c r="F2" s="75" t="s">
         <v>91</v>
       </c>
       <c r="G2" s="76" t="s">
+        <v>529</v>
+      </c>
+      <c r="H2" s="100" t="s">
         <v>530</v>
-      </c>
-      <c r="H2" s="100" t="s">
-        <v>531</v>
       </c>
       <c r="I2" s="100"/>
       <c r="J2" s="100" t="s">
+        <v>585</v>
+      </c>
+      <c r="K2" s="100" t="s">
         <v>586</v>
       </c>
-      <c r="K2" s="100" t="s">
-        <v>587</v>
-      </c>
       <c r="L2" s="100" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
       <c r="M2" s="100" t="s">
+        <v>582</v>
+      </c>
+      <c r="N2" s="100" t="s">
         <v>583</v>
       </c>
-      <c r="N2" s="100" t="s">
+      <c r="O2" s="100" t="s">
         <v>584</v>
       </c>
-      <c r="O2" s="100" t="s">
-        <v>585</v>
-      </c>
       <c r="P2" s="100" t="s">
+        <v>535</v>
+      </c>
+      <c r="Q2" s="100" t="s">
+        <v>591</v>
+      </c>
+      <c r="R2" s="100" t="s">
+        <v>592</v>
+      </c>
+      <c r="S2" s="100" t="s">
+        <v>593</v>
+      </c>
+      <c r="T2" s="100" t="s">
         <v>536</v>
       </c>
-      <c r="Q2" s="100" t="s">
-        <v>592</v>
-      </c>
-      <c r="R2" s="100" t="s">
-        <v>593</v>
-      </c>
-      <c r="S2" s="100" t="s">
-        <v>594</v>
-      </c>
-      <c r="T2" s="100" t="s">
-        <v>537</v>
-      </c>
       <c r="U2" s="100" t="s">
+        <v>598</v>
+      </c>
+      <c r="V2" s="100" t="s">
         <v>599</v>
       </c>
-      <c r="V2" s="100" t="s">
+      <c r="W2" s="100" t="s">
         <v>600</v>
       </c>
-      <c r="W2" s="100" t="s">
+      <c r="X2" s="100" t="s">
         <v>601</v>
       </c>
-      <c r="X2" s="100" t="s">
+      <c r="Y2" s="100" t="s">
         <v>602</v>
       </c>
-      <c r="Y2" s="100" t="s">
+      <c r="Z2" s="100" t="s">
         <v>603</v>
       </c>
-      <c r="Z2" s="100" t="s">
-        <v>604</v>
-      </c>
       <c r="AA2" s="100" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AB2" s="100" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AC2" s="100" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AD2" s="100"/>
       <c r="AE2" s="100" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="AF2" s="100" t="s">
+        <v>535</v>
+      </c>
+      <c r="AG2" s="100" t="s">
         <v>536</v>
       </c>
-      <c r="AG2" s="100" t="s">
-        <v>537</v>
-      </c>
       <c r="AH2" s="100" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
       <c r="AI2" s="100" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
       <c r="AJ2" s="100" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AK2" s="100" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AL2" s="100" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="AM2" s="100" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
       <c r="AN2" s="100" t="s">
+        <v>563</v>
+      </c>
+      <c r="AO2" s="100" t="s">
         <v>564</v>
-      </c>
-      <c r="AO2" s="100" t="s">
-        <v>565</v>
       </c>
     </row>
     <row r="3" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3357,10 +3357,10 @@
         <v>471</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>472</v>
@@ -3478,10 +3478,10 @@
         <v>471</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>476</v>
@@ -3599,10 +3599,10 @@
         <v>471</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>486</v>
@@ -3720,10 +3720,10 @@
         <v>471</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>477</v>
@@ -3835,22 +3835,22 @@
     </row>
     <row r="7" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>470</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E7" s="8" t="s">
+        <v>543</v>
+      </c>
+      <c r="F7" s="8" t="s">
         <v>544</v>
-      </c>
-      <c r="F7" s="8" t="s">
-        <v>545</v>
       </c>
       <c r="G7" s="51">
         <v>0</v>
@@ -3993,10 +3993,10 @@
         <v>470</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>129</v>
@@ -4114,10 +4114,10 @@
         <v>470</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>130</v>
@@ -4235,10 +4235,10 @@
         <v>470</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E10" s="75" t="s">
         <v>444</v>
@@ -4356,10 +4356,10 @@
         <v>470</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>114</v>
@@ -4477,10 +4477,10 @@
         <v>470</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>115</v>
@@ -4598,10 +4598,10 @@
         <v>470</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>123</v>
@@ -4719,10 +4719,10 @@
         <v>470</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>113</v>
@@ -4840,10 +4840,10 @@
         <v>470</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>448</v>
@@ -4961,10 +4961,10 @@
         <v>470</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>131</v>
@@ -5082,10 +5082,10 @@
         <v>470</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>116</v>
@@ -5203,10 +5203,10 @@
         <v>470</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>117</v>
@@ -5324,10 +5324,10 @@
         <v>470</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>455</v>
@@ -5445,10 +5445,10 @@
         <v>470</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>462</v>
@@ -5566,10 +5566,10 @@
         <v>470</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>465</v>
@@ -5687,10 +5687,10 @@
         <v>470</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>467</v>
@@ -5808,10 +5808,10 @@
         <v>470</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>133</v>
@@ -5929,10 +5929,10 @@
         <v>470</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>118</v>
@@ -6050,10 +6050,10 @@
         <v>470</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>363</v>
@@ -6171,10 +6171,10 @@
         <v>470</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>365</v>
@@ -6292,10 +6292,10 @@
         <v>470</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>377</v>
@@ -6413,10 +6413,10 @@
         <v>470</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>373</v>
@@ -6534,10 +6534,10 @@
         <v>470</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>372</v>
@@ -6655,10 +6655,10 @@
         <v>470</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>139</v>
@@ -6776,10 +6776,10 @@
         <v>470</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>119</v>
@@ -6897,10 +6897,10 @@
         <v>470</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>134</v>
@@ -7018,10 +7018,10 @@
         <v>470</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>132</v>
@@ -7139,10 +7139,10 @@
         <v>470</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>454</v>
@@ -7260,10 +7260,10 @@
         <v>470</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>137</v>
@@ -7381,10 +7381,10 @@
         <v>470</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>124</v>
@@ -7502,10 +7502,10 @@
         <v>470</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>125</v>
@@ -7623,10 +7623,10 @@
         <v>470</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>126</v>
@@ -7744,10 +7744,10 @@
         <v>470</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>138</v>
@@ -7865,10 +7865,10 @@
         <v>470</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>127</v>
@@ -7986,10 +7986,10 @@
         <v>470</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>128</v>
@@ -8107,10 +8107,10 @@
         <v>470</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>140</v>
@@ -8228,10 +8228,10 @@
         <v>470</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>141</v>
@@ -8349,10 +8349,10 @@
         <v>470</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>142</v>
@@ -8470,10 +8470,10 @@
         <v>470</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>143</v>
@@ -8591,10 +8591,10 @@
         <v>470</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>144</v>
@@ -8712,10 +8712,10 @@
         <v>470</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>145</v>
@@ -8833,10 +8833,10 @@
         <v>470</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>146</v>
@@ -8954,10 +8954,10 @@
         <v>470</v>
       </c>
       <c r="C49" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>147</v>
@@ -9075,10 +9075,10 @@
         <v>470</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>435</v>
@@ -9196,10 +9196,10 @@
         <v>470</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>436</v>
@@ -9317,10 +9317,10 @@
         <v>470</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>457</v>
@@ -9438,10 +9438,10 @@
         <v>470</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>135</v>
@@ -9559,10 +9559,10 @@
         <v>470</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>136</v>
@@ -9680,10 +9680,10 @@
         <v>470</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>120</v>
@@ -9801,10 +9801,10 @@
         <v>470</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>121</v>
@@ -9922,10 +9922,10 @@
         <v>470</v>
       </c>
       <c r="C57" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E57" s="12" t="s">
         <v>122</v>
@@ -10043,10 +10043,10 @@
         <v>470</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>148</v>
@@ -10164,10 +10164,10 @@
         <v>470</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>380</v>
@@ -10285,10 +10285,10 @@
         <v>470</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>149</v>
@@ -10406,10 +10406,10 @@
         <v>470</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>150</v>
@@ -10527,10 +10527,10 @@
         <v>470</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>151</v>
@@ -10648,10 +10648,10 @@
         <v>470</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>152</v>
@@ -10769,10 +10769,10 @@
         <v>470</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E64" s="18" t="s">
         <v>284</v>
@@ -10890,10 +10890,10 @@
         <v>470</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E65" s="18" t="s">
         <v>155</v>
@@ -11011,10 +11011,10 @@
         <v>470</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E66" s="18" t="s">
         <v>406</v>
@@ -11132,10 +11132,10 @@
         <v>470</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E67" s="18" t="s">
         <v>153</v>
@@ -11253,10 +11253,10 @@
         <v>470</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>408</v>
@@ -11374,10 +11374,10 @@
         <v>470</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E69" s="18" t="s">
         <v>154</v>
@@ -11495,10 +11495,10 @@
         <v>470</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E70" s="18" t="s">
         <v>288</v>
@@ -11616,10 +11616,10 @@
         <v>470</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>381</v>
@@ -11737,10 +11737,10 @@
         <v>470</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E72" s="18" t="s">
         <v>156</v>
@@ -11858,10 +11858,10 @@
         <v>470</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E73" s="18" t="s">
         <v>157</v>
@@ -11979,10 +11979,10 @@
         <v>470</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E74" s="18" t="s">
         <v>158</v>
@@ -12100,10 +12100,10 @@
         <v>470</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>159</v>
@@ -12221,10 +12221,10 @@
         <v>470</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E76" s="18" t="s">
         <v>160</v>
@@ -12342,10 +12342,10 @@
         <v>470</v>
       </c>
       <c r="C77" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E77" s="18" t="s">
         <v>161</v>
@@ -12463,10 +12463,10 @@
         <v>470</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E78" s="34" t="s">
         <v>418</v>
@@ -12584,10 +12584,10 @@
         <v>470</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E79" s="34" t="s">
         <v>412</v>
@@ -12705,10 +12705,10 @@
         <v>470</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E80" s="34" t="s">
         <v>419</v>
@@ -12826,10 +12826,10 @@
         <v>470</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E81" s="34" t="s">
         <v>402</v>
@@ -12947,10 +12947,10 @@
         <v>470</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E82" s="34" t="s">
         <v>415</v>
@@ -13068,10 +13068,10 @@
         <v>470</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E83" s="34" t="s">
         <v>414</v>
@@ -13189,10 +13189,10 @@
         <v>470</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E84" s="34" t="s">
         <v>416</v>
@@ -13310,10 +13310,10 @@
         <v>470</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E85" s="34" t="s">
         <v>403</v>
@@ -13431,10 +13431,10 @@
         <v>470</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E86" s="34" t="s">
         <v>404</v>
@@ -13552,10 +13552,10 @@
         <v>470</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E87" s="18" t="s">
         <v>162</v>
@@ -13673,10 +13673,10 @@
         <v>470</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E88" s="18" t="s">
         <v>163</v>
@@ -13794,10 +13794,10 @@
         <v>470</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E89" s="18" t="s">
         <v>164</v>
@@ -13915,10 +13915,10 @@
         <v>470</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E90" s="18" t="s">
         <v>165</v>
@@ -14036,10 +14036,10 @@
         <v>470</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E91" s="18" t="s">
         <v>166</v>
@@ -14157,10 +14157,10 @@
         <v>470</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E92" s="20" t="s">
         <v>290</v>
@@ -14278,10 +14278,10 @@
         <v>470</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>291</v>
@@ -14399,10 +14399,10 @@
         <v>470</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E94" s="20" t="s">
         <v>295</v>
@@ -14520,10 +14520,10 @@
         <v>470</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E95" s="20" t="s">
         <v>292</v>
@@ -14641,10 +14641,10 @@
         <v>470</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E96" s="20" t="s">
         <v>293</v>
@@ -14762,10 +14762,10 @@
         <v>470</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E97" s="14" t="s">
         <v>171</v>
@@ -14883,10 +14883,10 @@
         <v>470</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E98" s="14" t="s">
         <v>289</v>
@@ -15004,10 +15004,10 @@
         <v>470</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E99" s="14" t="s">
         <v>170</v>
@@ -15125,10 +15125,10 @@
         <v>470</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E100" s="24" t="s">
         <v>176</v>
@@ -15246,10 +15246,10 @@
         <v>470</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E101" s="24" t="s">
         <v>369</v>
@@ -15367,10 +15367,10 @@
         <v>470</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E102" s="24" t="s">
         <v>370</v>
@@ -15488,10 +15488,10 @@
         <v>470</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E103" s="24" t="s">
         <v>371</v>
@@ -15603,16 +15603,16 @@
     </row>
     <row r="104" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A104" s="23" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B104" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E104" s="24" t="s">
         <v>383</v>
@@ -15730,10 +15730,10 @@
         <v>470</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E105" s="24" t="s">
         <v>385</v>
@@ -15845,22 +15845,22 @@
     </row>
     <row r="106" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A106" s="23" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B106" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E106" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F106" s="24" t="s">
         <v>504</v>
-      </c>
-      <c r="F106" s="24" t="s">
-        <v>505</v>
       </c>
       <c r="G106" s="58">
         <f t="shared" ref="G106:H106" si="1">G104</f>
@@ -15999,22 +15999,22 @@
     </row>
     <row r="107" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A107" s="23" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B107" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E107" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F107" s="24" t="s">
         <v>504</v>
-      </c>
-      <c r="F107" s="24" t="s">
-        <v>505</v>
       </c>
       <c r="G107" s="58">
         <f>3*G104</f>
@@ -16153,22 +16153,22 @@
     </row>
     <row r="108" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A108" s="23" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="B108" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E108" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F108" s="24" t="s">
         <v>504</v>
-      </c>
-      <c r="F108" s="24" t="s">
-        <v>505</v>
       </c>
       <c r="G108" s="58">
         <f t="shared" ref="G108:H108" si="7">G99</f>
@@ -16307,22 +16307,22 @@
     </row>
     <row r="109" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A109" s="23" t="s">
-        <v>503</v>
+        <v>502</v>
       </c>
       <c r="B109" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E109" s="24" t="s">
+        <v>503</v>
+      </c>
+      <c r="F109" s="24" t="s">
         <v>504</v>
-      </c>
-      <c r="F109" s="24" t="s">
-        <v>505</v>
       </c>
       <c r="G109" s="58">
         <f>10*G99</f>
@@ -16467,10 +16467,10 @@
         <v>470</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E110" s="24" t="s">
         <v>387</v>
@@ -16588,10 +16588,10 @@
         <v>470</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E111" s="24" t="s">
         <v>389</v>
@@ -16709,10 +16709,10 @@
         <v>470</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E112" s="24" t="s">
         <v>391</v>
@@ -16830,10 +16830,10 @@
         <v>470</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E113" s="24" t="s">
         <v>393</v>
@@ -16951,10 +16951,10 @@
         <v>470</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E114" s="24" t="s">
         <v>421</v>
@@ -17072,10 +17072,10 @@
         <v>470</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E115" s="24" t="s">
         <v>423</v>
@@ -17226,10 +17226,10 @@
         <v>470</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E116" s="24" t="s">
         <v>425</v>
@@ -17374,16 +17374,16 @@
     </row>
     <row r="117" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A117" s="23" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B117" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E117" s="24" t="s">
         <v>426</v>
@@ -17495,16 +17495,16 @@
     </row>
     <row r="118" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A118" s="23" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B118" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E118" s="24" t="s">
         <v>427</v>
@@ -17649,16 +17649,16 @@
     </row>
     <row r="119" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A119" s="23" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B119" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E119" s="24" t="s">
         <v>428</v>
@@ -17809,10 +17809,10 @@
         <v>470</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E120" s="24" t="s">
         <v>395</v>
@@ -17930,10 +17930,10 @@
         <v>470</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E121" s="24" t="s">
         <v>397</v>
@@ -18051,10 +18051,10 @@
         <v>470</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E122" s="14" t="s">
         <v>172</v>
@@ -18172,10 +18172,10 @@
         <v>470</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E123" s="14" t="s">
         <v>173</v>
@@ -18325,10 +18325,10 @@
         <v>470</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E124" s="14" t="s">
         <v>174</v>
@@ -18446,10 +18446,10 @@
         <v>470</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E125" s="14" t="s">
         <v>175</v>
@@ -18567,10 +18567,10 @@
         <v>470</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E126" s="14" t="s">
         <v>450</v>
@@ -18688,10 +18688,10 @@
         <v>470</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E127" s="14" t="s">
         <v>452</v>
@@ -18809,10 +18809,10 @@
         <v>470</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E128" s="69" t="s">
         <v>178</v>
@@ -18928,10 +18928,10 @@
         <v>470</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E129" s="69" t="s">
         <v>441</v>
@@ -19047,10 +19047,10 @@
         <v>470</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E130" s="69" t="s">
         <v>446</v>
@@ -19168,10 +19168,10 @@
         <v>470</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E131" s="22" t="s">
         <v>177</v>
@@ -19289,10 +19289,10 @@
         <v>470</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E132" s="22" t="s">
         <v>438</v>
@@ -19410,10 +19410,10 @@
         <v>470</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E133" s="22" t="s">
         <v>311</v>
@@ -19531,10 +19531,10 @@
         <v>470</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E134" s="22" t="s">
         <v>312</v>
@@ -19652,10 +19652,10 @@
         <v>470</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E135" s="22" t="s">
         <v>313</v>
@@ -19773,10 +19773,10 @@
         <v>470</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E136" s="22" t="s">
         <v>314</v>
@@ -19894,10 +19894,10 @@
         <v>470</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E137" s="22" t="s">
         <v>178</v>
@@ -20015,10 +20015,10 @@
         <v>470</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E138" s="22" t="s">
         <v>315</v>
@@ -20136,10 +20136,10 @@
         <v>470</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E139" s="22" t="s">
         <v>316</v>
@@ -20257,10 +20257,10 @@
         <v>470</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E140" s="22" t="s">
         <v>317</v>
@@ -20378,10 +20378,10 @@
         <v>470</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E141" s="22" t="s">
         <v>318</v>
@@ -20499,10 +20499,10 @@
         <v>470</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E142" s="22" t="s">
         <v>180</v>
@@ -20620,10 +20620,10 @@
         <v>470</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E143" s="73" t="s">
         <v>181</v>
@@ -20741,10 +20741,10 @@
         <v>470</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E144" s="24" t="s">
         <v>167</v>
@@ -20862,10 +20862,10 @@
         <v>470</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E145" s="24" t="s">
         <v>168</v>
@@ -20983,10 +20983,10 @@
         <v>470</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E146" s="24" t="s">
         <v>169</v>
@@ -21104,10 +21104,10 @@
         <v>470</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E147" s="24" t="s">
         <v>183</v>
@@ -21225,10 +21225,10 @@
         <v>470</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E148" s="24" t="s">
         <v>303</v>
@@ -21346,10 +21346,10 @@
         <v>470</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E149" s="24" t="s">
         <v>304</v>
@@ -21467,10 +21467,10 @@
         <v>470</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E150" s="24" t="s">
         <v>305</v>
@@ -21588,10 +21588,10 @@
         <v>470</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E151" s="24" t="s">
         <v>306</v>
@@ -21709,10 +21709,10 @@
         <v>470</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E152" s="24" t="s">
         <v>184</v>
@@ -21830,10 +21830,10 @@
         <v>470</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E153" s="14" t="s">
         <v>186</v>
@@ -21951,10 +21951,10 @@
         <v>470</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E154" s="14" t="s">
         <v>307</v>
@@ -22072,10 +22072,10 @@
         <v>470</v>
       </c>
       <c r="C155" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E155" s="14" t="s">
         <v>308</v>
@@ -22193,10 +22193,10 @@
         <v>470</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E156" s="14" t="s">
         <v>309</v>
@@ -22314,10 +22314,10 @@
         <v>470</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E157" s="14" t="s">
         <v>310</v>
@@ -22435,10 +22435,10 @@
         <v>470</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E158" s="14" t="s">
         <v>185</v>
@@ -22556,10 +22556,10 @@
         <v>470</v>
       </c>
       <c r="C159" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>187</v>
@@ -22677,10 +22677,10 @@
         <v>470</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>298</v>
@@ -22798,10 +22798,10 @@
         <v>470</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E161" s="10" t="s">
         <v>299</v>
@@ -22919,10 +22919,10 @@
         <v>470</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E162" s="10" t="s">
         <v>300</v>
@@ -23040,10 +23040,10 @@
         <v>470</v>
       </c>
       <c r="C163" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E163" s="10" t="s">
         <v>302</v>
@@ -23161,10 +23161,10 @@
         <v>470</v>
       </c>
       <c r="C164" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E164" s="10" t="s">
         <v>188</v>
@@ -23282,10 +23282,10 @@
         <v>470</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E165" s="26" t="s">
         <v>189</v>
@@ -23403,10 +23403,10 @@
         <v>470</v>
       </c>
       <c r="C166" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E166" s="26" t="s">
         <v>319</v>
@@ -23524,10 +23524,10 @@
         <v>470</v>
       </c>
       <c r="C167" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E167" s="26" t="s">
         <v>320</v>
@@ -23645,10 +23645,10 @@
         <v>470</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E168" s="26" t="s">
         <v>321</v>
@@ -23766,10 +23766,10 @@
         <v>470</v>
       </c>
       <c r="C169" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E169" s="26" t="s">
         <v>322</v>
@@ -23887,10 +23887,10 @@
         <v>470</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E170" s="26" t="s">
         <v>190</v>
@@ -24008,10 +24008,10 @@
         <v>470</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E171" s="32" t="s">
         <v>191</v>
@@ -24129,10 +24129,10 @@
         <v>470</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E172" s="32" t="s">
         <v>323</v>
@@ -24250,10 +24250,10 @@
         <v>470</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E173" s="32" t="s">
         <v>324</v>
@@ -24371,10 +24371,10 @@
         <v>470</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E174" s="32" t="s">
         <v>325</v>
@@ -24492,10 +24492,10 @@
         <v>470</v>
       </c>
       <c r="C175" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E175" s="32" t="s">
         <v>326</v>
@@ -24613,10 +24613,10 @@
         <v>470</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E176" s="32" t="s">
         <v>192</v>
@@ -24734,10 +24734,10 @@
         <v>470</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E177" s="12" t="s">
         <v>327</v>
@@ -24855,10 +24855,10 @@
         <v>470</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E178" s="12" t="s">
         <v>329</v>
@@ -24976,10 +24976,10 @@
         <v>470</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E179" s="12" t="s">
         <v>330</v>
@@ -25097,10 +25097,10 @@
         <v>470</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E180" s="12" t="s">
         <v>331</v>
@@ -25218,10 +25218,10 @@
         <v>470</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E181" s="12" t="s">
         <v>332</v>
@@ -25339,10 +25339,10 @@
         <v>470</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E182" s="12" t="s">
         <v>349</v>
@@ -25460,10 +25460,10 @@
         <v>470</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E183" s="12" t="s">
         <v>350</v>
@@ -25581,10 +25581,10 @@
         <v>470</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E184" s="28" t="s">
         <v>351</v>
@@ -25702,10 +25702,10 @@
         <v>470</v>
       </c>
       <c r="C185" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E185" s="28" t="s">
         <v>333</v>
@@ -25823,10 +25823,10 @@
         <v>470</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E186" s="28" t="s">
         <v>334</v>
@@ -25944,10 +25944,10 @@
         <v>470</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E187" s="28" t="s">
         <v>335</v>
@@ -26065,10 +26065,10 @@
         <v>470</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E188" s="28" t="s">
         <v>336</v>
@@ -26186,10 +26186,10 @@
         <v>470</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E189" s="28" t="s">
         <v>353</v>
@@ -26307,10 +26307,10 @@
         <v>470</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E190" s="24" t="s">
         <v>193</v>
@@ -26428,10 +26428,10 @@
         <v>470</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E191" s="24" t="s">
         <v>337</v>
@@ -26549,10 +26549,10 @@
         <v>470</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E192" s="24" t="s">
         <v>338</v>
@@ -26670,10 +26670,10 @@
         <v>470</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E193" s="24" t="s">
         <v>339</v>
@@ -26791,10 +26791,10 @@
         <v>470</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E194" s="24" t="s">
         <v>340</v>
@@ -26912,10 +26912,10 @@
         <v>470</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E195" s="24" t="s">
         <v>194</v>
@@ -27033,10 +27033,10 @@
         <v>470</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>355</v>
@@ -27154,10 +27154,10 @@
         <v>470</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>341</v>
@@ -27275,10 +27275,10 @@
         <v>470</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>342</v>
@@ -27396,10 +27396,10 @@
         <v>470</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>343</v>
@@ -27517,10 +27517,10 @@
         <v>470</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>344</v>
@@ -27638,10 +27638,10 @@
         <v>470</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>358</v>
@@ -27759,10 +27759,10 @@
         <v>470</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E202" s="30" t="s">
         <v>356</v>
@@ -27880,10 +27880,10 @@
         <v>470</v>
       </c>
       <c r="C203" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E203" s="30" t="s">
         <v>345</v>
@@ -28001,10 +28001,10 @@
         <v>470</v>
       </c>
       <c r="C204" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E204" s="30" t="s">
         <v>346</v>
@@ -28122,10 +28122,10 @@
         <v>470</v>
       </c>
       <c r="C205" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E205" s="30" t="s">
         <v>347</v>
@@ -28243,10 +28243,10 @@
         <v>470</v>
       </c>
       <c r="C206" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E206" s="30" t="s">
         <v>348</v>
@@ -28364,10 +28364,10 @@
         <v>470</v>
       </c>
       <c r="C207" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E207" s="30" t="s">
         <v>360</v>
@@ -28485,10 +28485,10 @@
         <v>470</v>
       </c>
       <c r="C208" s="92" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E208" s="93" t="s">
         <v>203</v>
@@ -28600,16 +28600,16 @@
     </row>
     <row r="209" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C209" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E209" s="30" t="s">
         <v>491</v>
@@ -28621,68 +28621,89 @@
         <v>0.5</v>
       </c>
       <c r="H209" s="2">
-        <v>2.2000000000000002</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="I209" s="2"/>
       <c r="J209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="K209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="L209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="M209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="N209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="O209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="P209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="Q209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="R209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="S209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="T209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="U209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="V209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="W209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="X209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="Y209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="Z209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="AA209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="AB209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="AC209" s="2">
-        <v>1.36</v>
+        <f>0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="AD209" s="2"/>
       <c r="AE209" s="2">
@@ -28727,89 +28748,89 @@
     </row>
     <row r="210" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>493</v>
+        <v>619</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C210" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E210" s="30" t="s">
+        <v>493</v>
+      </c>
+      <c r="F210" s="30" t="s">
         <v>494</v>
-      </c>
-      <c r="F210" s="30" t="s">
-        <v>495</v>
       </c>
       <c r="G210" s="97">
         <v>-100000</v>
       </c>
       <c r="H210" s="98">
-        <v>-100000</v>
+        <v>0.25</v>
       </c>
       <c r="I210" s="98"/>
       <c r="J210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="K210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="L210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="M210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="N210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="O210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="P210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="Q210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="R210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="S210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="T210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="U210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="V210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="W210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="X210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="Y210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="Z210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="AA210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="AB210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="AC210" s="98">
-        <v>-30000</v>
+        <v>0.25</v>
       </c>
       <c r="AD210" s="98"/>
       <c r="AE210" s="98">
@@ -28848,28 +28869,27 @@
     </row>
     <row r="211" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="B211" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E211" s="30" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F211" s="30" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="G211" s="97">
         <v>-100000</v>
       </c>
       <c r="H211" s="98">
-        <f t="shared" ref="H211" si="19">H210</f>
         <v>-100000</v>
       </c>
       <c r="I211" s="98"/>
@@ -28970,19 +28990,19 @@
     </row>
     <row r="212" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C212" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E212" s="96" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="F212" s="96" t="s">
         <v>490</v>
@@ -29091,22 +29111,22 @@
     </row>
     <row r="213" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="B213" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C213" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E213" s="96" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F213" s="96" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G213" s="99" t="s">
         <v>474</v>
@@ -29212,22 +29232,22 @@
     </row>
     <row r="214" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="B214" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C214" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E214" s="96" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="F214" s="96" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G214" s="99">
         <v>0</v>
@@ -29333,22 +29353,22 @@
     </row>
     <row r="215" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="B215" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C215" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E215" s="96" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F215" s="96" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G215" s="99">
         <v>1E-3</v>
@@ -29454,22 +29474,22 @@
     </row>
     <row r="216" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="B216" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C216" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E216" s="96" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F216" s="96" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G216" s="99">
         <v>29</v>
@@ -29575,176 +29595,176 @@
     </row>
     <row r="217" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="B217" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C217" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E217" s="96" t="s">
+        <v>518</v>
+      </c>
+      <c r="F217" s="96" t="s">
         <v>519</v>
-      </c>
-      <c r="F217" s="96" t="s">
-        <v>520</v>
       </c>
       <c r="G217" s="98">
         <f>1.25*0.000001</f>
         <v>1.2499999999999999E-6</v>
       </c>
       <c r="H217" s="98">
-        <f t="shared" ref="H217:AO217" si="20">1250*0.000001/5</f>
+        <f t="shared" ref="H217:AO217" si="19">1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="I217" s="98"/>
       <c r="J217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="L217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="M217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="N217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="O217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="P217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="R217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="S217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="T217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="U217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="V217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="W217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="X217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Y217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Z217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AA217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AB217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AC217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AD217" s="98"/>
       <c r="AE217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AF217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AG217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AH217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AI217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AJ217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AK217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AL217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AM217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AN217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AO217" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="19"/>
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
     <row r="218" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="B218" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C218" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E218" s="96" t="s">
+        <v>523</v>
+      </c>
+      <c r="F218" s="96" t="s">
         <v>524</v>
-      </c>
-      <c r="F218" s="96" t="s">
-        <v>525</v>
       </c>
       <c r="G218" s="98">
         <v>2.0000000000000001E-4</v>
@@ -29850,22 +29870,22 @@
     </row>
     <row r="219" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C219" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E219" s="96" t="s">
+        <v>552</v>
+      </c>
+      <c r="F219" s="96" t="s">
         <v>553</v>
-      </c>
-      <c r="F219" s="96" t="s">
-        <v>554</v>
       </c>
       <c r="G219" s="98">
         <v>2.4999999999999998E-12</v>
@@ -29971,22 +29991,22 @@
     </row>
     <row r="220" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C220" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E220" s="96" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="F220" s="96" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="G220" s="98">
         <v>1.2E-8</v>
@@ -30092,22 +30112,22 @@
     </row>
     <row r="221" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C221" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E221" s="96" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="F221" s="96" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G221" s="98">
         <v>9.9999999999999995E-8</v>
@@ -30213,22 +30233,22 @@
     </row>
     <row r="222" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C222" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E222" s="96" t="s">
+        <v>557</v>
+      </c>
+      <c r="F222" s="96" t="s">
         <v>558</v>
-      </c>
-      <c r="F222" s="96" t="s">
-        <v>559</v>
       </c>
       <c r="G222" s="98">
         <f>2*0.00001</f>
@@ -30336,22 +30356,22 @@
     </row>
     <row r="223" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="B223" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C223" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E223" s="96" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F223" s="96" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="G223" s="98">
         <f>0.00000000000001 * 1000</f>
@@ -30363,149 +30383,149 @@
       </c>
       <c r="I223" s="98"/>
       <c r="J223" s="98">
-        <f t="shared" ref="J223:AO223" si="21">0.00000000000001*10000*8</f>
+        <f t="shared" ref="J223:AO223" si="20">0.00000000000001*10000*8</f>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="K223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="L223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="M223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="N223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="O223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="P223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="Q223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="R223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="S223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="T223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="U223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="V223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="W223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="X223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="Y223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="Z223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AA223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AB223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AC223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AD223" s="98"/>
       <c r="AE223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AF223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AG223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AH223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AI223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AJ223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AK223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AL223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AM223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AN223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AO223" s="98">
-        <f t="shared" si="21"/>
+        <f t="shared" si="20"/>
         <v>8.0000000000000003E-10</v>
       </c>
     </row>
     <row r="224" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C224" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E224" s="96" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="F224" s="96" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="G224" s="98">
         <f>0.00000000000001 * 10000</f>
@@ -30517,149 +30537,149 @@
       </c>
       <c r="I224" s="98"/>
       <c r="J224" s="98">
-        <f t="shared" ref="J224:K224" si="22">J223*10</f>
+        <f t="shared" ref="J224:K224" si="21">J223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="K224" s="98">
+        <f t="shared" si="21"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="L224" s="98">
+        <f t="shared" ref="L224:N224" si="22">L223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="M224" s="98">
         <f t="shared" si="22"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="L224" s="98">
-        <f t="shared" ref="L224:N224" si="23">L223*10</f>
+      <c r="N224" s="98">
+        <f t="shared" si="22"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="M224" s="98">
+      <c r="O224" s="98">
+        <f t="shared" ref="O224:R224" si="23">O223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="P224" s="98">
         <f t="shared" si="23"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="N224" s="98">
+      <c r="Q224" s="98">
         <f t="shared" si="23"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="O224" s="98">
-        <f t="shared" ref="O224:R224" si="24">O223*10</f>
+      <c r="R224" s="98">
+        <f t="shared" si="23"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="P224" s="98">
+      <c r="S224" s="98">
+        <f t="shared" ref="S224:V224" si="24">S223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="T224" s="98">
         <f t="shared" si="24"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="Q224" s="98">
+      <c r="U224" s="98">
         <f t="shared" si="24"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="R224" s="98">
+      <c r="V224" s="98">
         <f t="shared" si="24"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="S224" s="98">
-        <f t="shared" ref="S224:V224" si="25">S223*10</f>
+      <c r="W224" s="98">
+        <f t="shared" ref="W224:AA224" si="25">W223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="T224" s="98">
+      <c r="X224" s="98">
         <f t="shared" si="25"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="U224" s="98">
+      <c r="Y224" s="98">
         <f t="shared" si="25"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="V224" s="98">
+      <c r="Z224" s="98">
         <f t="shared" si="25"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="W224" s="98">
-        <f t="shared" ref="W224:AA224" si="26">W223*10</f>
+      <c r="AA224" s="98">
+        <f t="shared" si="25"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="X224" s="98">
+      <c r="AB224" s="98">
+        <f t="shared" ref="AB224:AC224" si="26">AB223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="AC224" s="98">
         <f t="shared" si="26"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="Y224" s="98">
-        <f t="shared" si="26"/>
+      <c r="AD224" s="98"/>
+      <c r="AE224" s="98">
+        <f t="shared" ref="AE224:AO224" si="27">AE223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="Z224" s="98">
-        <f t="shared" si="26"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="AA224" s="98">
-        <f t="shared" si="26"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="AB224" s="98">
-        <f t="shared" ref="AB224:AC224" si="27">AB223*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="AC224" s="98">
+      <c r="AF224" s="98">
         <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AD224" s="98"/>
-      <c r="AE224" s="98">
-        <f t="shared" ref="AE224:AO224" si="28">AE223*10</f>
+      <c r="AG224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AF224" s="98">
-        <f t="shared" si="28"/>
+      <c r="AH224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AG224" s="98">
-        <f t="shared" si="28"/>
+      <c r="AI224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AH224" s="98">
-        <f t="shared" si="28"/>
+      <c r="AJ224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AI224" s="98">
-        <f t="shared" si="28"/>
+      <c r="AK224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AJ224" s="98">
-        <f t="shared" si="28"/>
+      <c r="AL224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AK224" s="98">
-        <f t="shared" si="28"/>
+      <c r="AM224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AL224" s="98">
-        <f t="shared" si="28"/>
+      <c r="AN224" s="98">
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="AM224" s="98">
-        <f t="shared" si="28"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="AN224" s="98">
-        <f t="shared" si="28"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
       <c r="AO224" s="98">
-        <f t="shared" si="28"/>
+        <f t="shared" si="27"/>
         <v>8.0000000000000005E-9</v>
       </c>
     </row>
     <row r="225" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C225" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E225" s="96" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F225" s="96" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="G225" s="98">
         <f>0.84*(0.36^2)</f>
@@ -30767,19 +30787,19 @@
     </row>
     <row r="226" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C226" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E226" s="96" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F226" s="96" t="s">
         <v>490</v>
@@ -30888,22 +30908,22 @@
     </row>
     <row r="227" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C227" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E227" s="96" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F227" s="96" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G227" s="99" t="s">
         <v>474</v>
@@ -31009,22 +31029,22 @@
     </row>
     <row r="228" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C228" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E228" s="96" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F228" s="96" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G228" s="99">
         <f>2*0.1</f>
@@ -31036,149 +31056,149 @@
       </c>
       <c r="I228" s="99"/>
       <c r="J228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" ref="J228:AC228" si="28">2*0.1</f>
         <v>0.2</v>
       </c>
       <c r="K228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="L228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="M228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="N228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="O228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="P228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="Q228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="R228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="S228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="T228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="U228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="V228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="W228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="X228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="Y228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="Z228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="AA228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="AB228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="AC228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="28"/>
         <v>0.2</v>
       </c>
       <c r="AD228" s="99"/>
       <c r="AE228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" ref="AE228:AO228" si="29">2*0.1</f>
         <v>0.2</v>
       </c>
       <c r="AF228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AG228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AH228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AI228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AJ228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AK228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AL228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AM228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AN228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
       <c r="AO228" s="99">
-        <f>2*0.1</f>
+        <f t="shared" si="29"/>
         <v>0.2</v>
       </c>
     </row>
     <row r="229" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>470</v>
       </c>
       <c r="C229" s="2" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="E229" s="96" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="F229" s="96" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G229" s="99">
         <v>1E-3</v>

</xml_diff>

<commit_message>
added output check file
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_09_22.xlsx
+++ b/simulations/inputs/Scenarios_24_09_22.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D980FE-CBD5-4C85-BF26-9ED0F467DA37}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD78FC-EB29-4EB2-9D76-2B1A9BC7DB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2923" uniqueCount="620">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2929" uniqueCount="622">
   <si>
     <t>input_file</t>
   </si>
@@ -1894,6 +1894,12 @@
   </si>
   <si>
     <t>soil_moisture</t>
+  </si>
+  <si>
+    <t>smax_AA</t>
+  </si>
+  <si>
+    <t>Maximal rate of amino acid synthesis in the root segment</t>
   </si>
 </sst>
 </file>
@@ -3086,13 +3092,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AO229"/>
+  <dimension ref="A1:AO230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="7" ySplit="1" topLeftCell="H181" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K213" sqref="K213"/>
+      <selection pane="bottomRight" activeCell="L228" sqref="L228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28626,84 +28632,84 @@
       </c>
       <c r="I209" s="2"/>
       <c r="J209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" ref="J209:K209" si="18">0.00002 / 14 / 5</f>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="K209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="18"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="L209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f>0.00002 / 14 / 5</f>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="M209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" ref="M209:AC209" si="19">0.00002 / 14 / 5</f>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="N209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="O209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="P209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="Q209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="R209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="S209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="T209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="U209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="V209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="W209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="X209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="Y209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="Z209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="AA209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="AB209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="AC209" s="2">
-        <f>0.00002 / 14</f>
-        <v>1.4285714285714286E-6</v>
+        <f t="shared" si="19"/>
+        <v>2.8571428571428575E-7</v>
       </c>
       <c r="AD209" s="2"/>
       <c r="AE209" s="2">
@@ -28722,27 +28728,27 @@
         <v>1.36</v>
       </c>
       <c r="AJ209" s="2">
-        <f t="shared" ref="AJ209:AO209" si="18">1.36+20</f>
+        <f t="shared" ref="AJ209:AO209" si="20">1.36+20</f>
         <v>21.36</v>
       </c>
       <c r="AK209" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>21.36</v>
       </c>
       <c r="AL209" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>21.36</v>
       </c>
       <c r="AM209" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>21.36</v>
       </c>
       <c r="AN209" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>21.36</v>
       </c>
       <c r="AO209" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>21.36</v>
       </c>
     </row>
@@ -28773,64 +28779,64 @@
       </c>
       <c r="I210" s="98"/>
       <c r="J210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="K210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="L210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="M210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="N210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="O210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="P210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="Q210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="R210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="S210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="T210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="U210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="V210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="W210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="X210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="Y210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="Z210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="AA210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="AB210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="AC210" s="98">
-        <v>0.25</v>
+        <v>0.3</v>
       </c>
       <c r="AD210" s="98"/>
       <c r="AE210" s="98">
@@ -29014,65 +29020,85 @@
         <v>0.5</v>
       </c>
       <c r="I212" s="99"/>
-      <c r="J212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="K212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="L212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="M212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="N212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="O212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="P212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="Q212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="R212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="S212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="T212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="U212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="V212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="W212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="X212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="Y212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="Z212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="AA212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="AB212" s="99">
-        <v>0.5</v>
-      </c>
-      <c r="AC212" s="99">
-        <v>0.5</v>
+      <c r="J212" s="2">
+        <f t="shared" ref="J212:AC212" si="21">0.00002 / 14</f>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="K212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="L212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="M212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="N212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="O212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="P212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="Q212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="R212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="S212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="T212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="U212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="V212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="W212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="X212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="Y212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="Z212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="AA212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="AB212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
+      </c>
+      <c r="AC212" s="2">
+        <f t="shared" si="21"/>
+        <v>1.4285714285714286E-6</v>
       </c>
       <c r="AD212" s="99"/>
       <c r="AE212" s="99">
@@ -29257,64 +29283,64 @@
       </c>
       <c r="I214" s="99"/>
       <c r="J214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="K214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="L214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="M214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="N214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="O214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="P214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="Q214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="R214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="S214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="T214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="U214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="V214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="W214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="X214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="Y214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="Z214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="AA214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="AB214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="AC214" s="99">
-        <v>0</v>
+        <v>0.15</v>
       </c>
       <c r="AD214" s="99"/>
       <c r="AE214" s="99">
@@ -29617,133 +29643,133 @@
         <v>1.2499999999999999E-6</v>
       </c>
       <c r="H217" s="98">
-        <f t="shared" ref="H217:AO217" si="19">1250*0.000001/5</f>
+        <f t="shared" ref="H217:AO217" si="22">1250*0.000001/5</f>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="I217" s="98"/>
       <c r="J217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="K217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="L217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="M217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="N217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="O217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="P217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Q217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="R217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="S217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="T217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="U217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="V217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="W217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="X217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Y217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="Z217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AA217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AB217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AC217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AD217" s="98"/>
       <c r="AE217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AF217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AG217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AH217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AI217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AJ217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AK217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AL217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AM217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AN217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
       <c r="AO217" s="98">
-        <f t="shared" si="19"/>
+        <f t="shared" si="22"/>
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
@@ -30016,64 +30042,84 @@
       </c>
       <c r="I220" s="98"/>
       <c r="J220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" ref="J220:AC220" si="23">0.00000012*100</f>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="K220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="L220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="M220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="N220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="O220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="P220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="Q220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="R220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="S220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="T220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="U220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="V220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="W220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="X220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="Y220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="Z220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="AA220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="AB220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="AC220" s="98">
-        <v>1.1999999999999999E-7</v>
+        <f t="shared" si="23"/>
+        <v>1.1999999999999999E-5</v>
       </c>
       <c r="AD220" s="98"/>
       <c r="AE220" s="98">
@@ -30383,128 +30429,128 @@
       </c>
       <c r="I223" s="98"/>
       <c r="J223" s="98">
-        <f t="shared" ref="J223:AO223" si="20">0.00000000000001*10000*8</f>
+        <f t="shared" ref="J223:AO223" si="24">0.00000000000001*10000*8</f>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="K223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="L223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="M223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="N223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="O223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="P223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="Q223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="R223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="S223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="T223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="U223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="V223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="W223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="X223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="Y223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="Z223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AA223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AB223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AC223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AD223" s="98"/>
       <c r="AE223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AF223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AG223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AH223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AI223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AJ223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AK223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AL223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AM223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AN223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AO223" s="98">
-        <f t="shared" si="20"/>
+        <f t="shared" si="24"/>
         <v>8.0000000000000003E-10</v>
       </c>
     </row>
@@ -30537,128 +30583,128 @@
       </c>
       <c r="I224" s="98"/>
       <c r="J224" s="98">
-        <f t="shared" ref="J224:K224" si="21">J223*10</f>
+        <f t="shared" ref="J224:K224" si="25">J223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="K224" s="98">
-        <f t="shared" si="21"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="L224" s="98">
-        <f t="shared" ref="L224:N224" si="22">L223*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="M224" s="98">
-        <f t="shared" si="22"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="N224" s="98">
-        <f t="shared" si="22"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="O224" s="98">
-        <f t="shared" ref="O224:R224" si="23">O223*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="P224" s="98">
-        <f t="shared" si="23"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="Q224" s="98">
-        <f t="shared" si="23"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="R224" s="98">
-        <f t="shared" si="23"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="S224" s="98">
-        <f t="shared" ref="S224:V224" si="24">S223*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="T224" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="U224" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="V224" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="W224" s="98">
-        <f t="shared" ref="W224:AA224" si="25">W223*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="X224" s="98">
         <f t="shared" si="25"/>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="Y224" s="98">
-        <f t="shared" si="25"/>
+      <c r="L224" s="98">
+        <f t="shared" ref="L224:N224" si="26">L223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
-      <c r="Z224" s="98">
-        <f t="shared" si="25"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="AA224" s="98">
-        <f t="shared" si="25"/>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="AB224" s="98">
-        <f t="shared" ref="AB224:AC224" si="26">AB223*10</f>
-        <v>8.0000000000000005E-9</v>
-      </c>
-      <c r="AC224" s="98">
+      <c r="M224" s="98">
         <f t="shared" si="26"/>
         <v>8.0000000000000005E-9</v>
       </c>
+      <c r="N224" s="98">
+        <f t="shared" si="26"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="O224" s="98">
+        <f t="shared" ref="O224:R224" si="27">O223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="P224" s="98">
+        <f t="shared" si="27"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="Q224" s="98">
+        <f t="shared" si="27"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="R224" s="98">
+        <f t="shared" si="27"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="S224" s="98">
+        <f t="shared" ref="S224:V224" si="28">S223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="T224" s="98">
+        <f t="shared" si="28"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="U224" s="98">
+        <f t="shared" si="28"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="V224" s="98">
+        <f t="shared" si="28"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="W224" s="98">
+        <f t="shared" ref="W224:AA224" si="29">W223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="X224" s="98">
+        <f t="shared" si="29"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="Y224" s="98">
+        <f t="shared" si="29"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="Z224" s="98">
+        <f t="shared" si="29"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="AA224" s="98">
+        <f t="shared" si="29"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="AB224" s="98">
+        <f t="shared" ref="AB224:AC224" si="30">AB223*10</f>
+        <v>8.0000000000000005E-9</v>
+      </c>
+      <c r="AC224" s="98">
+        <f t="shared" si="30"/>
+        <v>8.0000000000000005E-9</v>
+      </c>
       <c r="AD224" s="98"/>
       <c r="AE224" s="98">
-        <f t="shared" ref="AE224:AO224" si="27">AE223*10</f>
+        <f t="shared" ref="AE224:AO224" si="31">AE223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AF224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AG224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AH224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AI224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AJ224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AK224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AL224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AM224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AN224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AO224" s="98">
-        <f t="shared" si="27"/>
+        <f t="shared" si="31"/>
         <v>8.0000000000000005E-9</v>
       </c>
     </row>
@@ -30812,64 +30858,64 @@
       </c>
       <c r="I226" s="99"/>
       <c r="J226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="K226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="L226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="M226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="N226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="O226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="P226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="Q226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="R226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="S226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="T226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="U226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="V226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="W226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="X226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="Y226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="Z226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AA226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AB226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AC226" s="99">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="AD226" s="99"/>
       <c r="AE226" s="99">
@@ -31056,128 +31102,128 @@
       </c>
       <c r="I228" s="99"/>
       <c r="J228" s="99">
-        <f t="shared" ref="J228:AC228" si="28">2*0.1</f>
-        <v>0.2</v>
+        <f t="shared" ref="J228:K228" si="32">2*0.075</f>
+        <v>0.15</v>
       </c>
       <c r="K228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="32"/>
+        <v>0.15</v>
       </c>
       <c r="L228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f>2*0.075</f>
+        <v>0.15</v>
       </c>
       <c r="M228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" ref="M228:AC228" si="33">2*0.075</f>
+        <v>0.15</v>
       </c>
       <c r="N228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="O228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="P228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="Q228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="R228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="S228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="T228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="U228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="V228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="W228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="X228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="Y228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="Z228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="AA228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="AB228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="AC228" s="99">
-        <f t="shared" si="28"/>
-        <v>0.2</v>
+        <f t="shared" si="33"/>
+        <v>0.15</v>
       </c>
       <c r="AD228" s="99"/>
       <c r="AE228" s="99">
-        <f t="shared" ref="AE228:AO228" si="29">2*0.1</f>
+        <f t="shared" ref="AE228:AO228" si="34">2*0.1</f>
         <v>0.2</v>
       </c>
       <c r="AF228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AG228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AH228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AI228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AJ228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AK228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AL228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AM228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AN228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
       <c r="AO228" s="99">
-        <f t="shared" si="29"/>
+        <f t="shared" si="34"/>
         <v>0.2</v>
       </c>
     </row>
@@ -31300,6 +31346,156 @@
       </c>
       <c r="AO229" s="99">
         <v>1E-3</v>
+      </c>
+    </row>
+    <row r="230" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A230" s="2" t="s">
+        <v>620</v>
+      </c>
+      <c r="B230" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="C230" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="D230" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="E230" s="96" t="s">
+        <v>621</v>
+      </c>
+      <c r="F230" s="96" t="s">
+        <v>508</v>
+      </c>
+      <c r="G230" s="97">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="H230" s="97">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="J230" s="97">
+        <f t="shared" ref="J230:AC230" si="35">0.00001*10</f>
+        <v>1E-4</v>
+      </c>
+      <c r="K230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="L230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="M230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="N230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="O230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="P230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="Q230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="R230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="S230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="T230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="U230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="V230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="W230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="X230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="Y230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="Z230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="AA230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="AB230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="AC230" s="97">
+        <f t="shared" si="35"/>
+        <v>1E-4</v>
+      </c>
+      <c r="AE230" s="97">
+        <f t="shared" ref="AE230:AO230" si="36">0.00001</f>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AF230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AG230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AH230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AI230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AJ230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AK230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AL230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AM230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AN230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="AO230" s="97">
+        <f t="shared" si="36"/>
+        <v>1.0000000000000001E-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
corrected the way deficits are computed to avoid inter timestep delays
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_09_22.xlsx
+++ b/simulations/inputs/Scenarios_24_09_22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16AD78FC-EB29-4EB2-9D76-2B1A9BC7DB51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B483C5F9-30DC-4194-A959-461CE8572CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_as_columns" sheetId="2" r:id="rId1"/>
@@ -1668,9 +1668,6 @@
     <t>Plant age to be used to start reading input tables in case of starting after seeding</t>
   </si>
   <si>
-    <t>second</t>
-  </si>
-  <si>
     <t>Input_RSML_HN_D13</t>
   </si>
   <si>
@@ -1900,6 +1897,9 @@
   </si>
   <si>
     <t>Maximal rate of amino acid synthesis in the root segment</t>
+  </si>
+  <si>
+    <t>hours</t>
   </si>
 </sst>
 </file>
@@ -2773,48 +2773,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3095,13 +3095,13 @@
   <dimension ref="A1:AO230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H181" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="H189" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L228" sqref="L228"/>
+      <selection pane="bottomRight" activeCell="J209" sqref="J209:J210"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
     <col min="2" max="4" width="15" style="1" customWidth="1"/>
@@ -3140,64 +3140,64 @@
       </c>
       <c r="I1" s="36"/>
       <c r="J1" s="36" t="s">
+        <v>574</v>
+      </c>
+      <c r="K1" s="36" t="s">
         <v>575</v>
       </c>
-      <c r="K1" s="36" t="s">
+      <c r="L1" s="36" t="s">
         <v>576</v>
       </c>
-      <c r="L1" s="36" t="s">
+      <c r="M1" s="36" t="s">
         <v>577</v>
       </c>
-      <c r="M1" s="36" t="s">
+      <c r="N1" s="36" t="s">
         <v>578</v>
       </c>
-      <c r="N1" s="36" t="s">
+      <c r="O1" s="36" t="s">
         <v>579</v>
       </c>
-      <c r="O1" s="36" t="s">
+      <c r="P1" s="36" t="s">
         <v>580</v>
       </c>
-      <c r="P1" s="36" t="s">
-        <v>581</v>
-      </c>
       <c r="Q1" s="36" t="s">
+        <v>586</v>
+      </c>
+      <c r="R1" s="36" t="s">
         <v>587</v>
       </c>
-      <c r="R1" s="36" t="s">
+      <c r="S1" s="36" t="s">
         <v>588</v>
       </c>
-      <c r="S1" s="36" t="s">
+      <c r="T1" s="36" t="s">
         <v>589</v>
       </c>
-      <c r="T1" s="36" t="s">
-        <v>590</v>
-      </c>
       <c r="U1" s="36" t="s">
+        <v>594</v>
+      </c>
+      <c r="V1" s="36" t="s">
         <v>595</v>
       </c>
-      <c r="V1" s="36" t="s">
+      <c r="W1" s="36" t="s">
         <v>596</v>
       </c>
-      <c r="W1" s="36" t="s">
-        <v>597</v>
-      </c>
       <c r="X1" s="36" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
       <c r="Y1" s="36" t="s">
+        <v>603</v>
+      </c>
+      <c r="Z1" s="36" t="s">
         <v>604</v>
       </c>
-      <c r="Z1" s="36" t="s">
+      <c r="AA1" s="36" t="s">
         <v>605</v>
       </c>
-      <c r="AA1" s="36" t="s">
+      <c r="AB1" s="36" t="s">
         <v>606</v>
       </c>
-      <c r="AB1" s="36" t="s">
+      <c r="AC1" s="36" t="s">
         <v>607</v>
-      </c>
-      <c r="AC1" s="36" t="s">
-        <v>608</v>
       </c>
       <c r="AD1" s="36"/>
       <c r="AE1" s="36" t="s">
@@ -3216,22 +3216,22 @@
         <v>540</v>
       </c>
       <c r="AJ1" s="36" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
       <c r="AK1" s="36" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
       <c r="AL1" s="36" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="AM1" s="36" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
       <c r="AN1" s="36" t="s">
+        <v>560</v>
+      </c>
+      <c r="AO1" s="36" t="s">
         <v>561</v>
-      </c>
-      <c r="AO1" s="36" t="s">
-        <v>562</v>
       </c>
     </row>
     <row r="2" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -3245,7 +3245,7 @@
         <v>525</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E2" s="75" t="s">
         <v>528</v>
@@ -3261,55 +3261,55 @@
       </c>
       <c r="I2" s="100"/>
       <c r="J2" s="100" t="s">
+        <v>584</v>
+      </c>
+      <c r="K2" s="100" t="s">
         <v>585</v>
-      </c>
-      <c r="K2" s="100" t="s">
-        <v>586</v>
       </c>
       <c r="L2" s="100" t="s">
         <v>531</v>
       </c>
       <c r="M2" s="100" t="s">
+        <v>581</v>
+      </c>
+      <c r="N2" s="100" t="s">
         <v>582</v>
       </c>
-      <c r="N2" s="100" t="s">
+      <c r="O2" s="100" t="s">
         <v>583</v>
-      </c>
-      <c r="O2" s="100" t="s">
-        <v>584</v>
       </c>
       <c r="P2" s="100" t="s">
         <v>535</v>
       </c>
       <c r="Q2" s="100" t="s">
+        <v>590</v>
+      </c>
+      <c r="R2" s="100" t="s">
         <v>591</v>
       </c>
-      <c r="R2" s="100" t="s">
+      <c r="S2" s="100" t="s">
         <v>592</v>
-      </c>
-      <c r="S2" s="100" t="s">
-        <v>593</v>
       </c>
       <c r="T2" s="100" t="s">
         <v>536</v>
       </c>
       <c r="U2" s="100" t="s">
+        <v>597</v>
+      </c>
+      <c r="V2" s="100" t="s">
         <v>598</v>
       </c>
-      <c r="V2" s="100" t="s">
+      <c r="W2" s="100" t="s">
         <v>599</v>
       </c>
-      <c r="W2" s="100" t="s">
+      <c r="X2" s="100" t="s">
         <v>600</v>
       </c>
-      <c r="X2" s="100" t="s">
+      <c r="Y2" s="100" t="s">
         <v>601</v>
       </c>
-      <c r="Y2" s="100" t="s">
+      <c r="Z2" s="100" t="s">
         <v>602</v>
-      </c>
-      <c r="Z2" s="100" t="s">
-        <v>603</v>
       </c>
       <c r="AA2" s="100" t="s">
         <v>539</v>
@@ -3337,22 +3337,22 @@
         <v>541</v>
       </c>
       <c r="AJ2" s="100" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
       <c r="AK2" s="100" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="AL2" s="100" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
       <c r="AM2" s="100" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="AN2" s="100" t="s">
+        <v>562</v>
+      </c>
+      <c r="AO2" s="100" t="s">
         <v>563</v>
-      </c>
-      <c r="AO2" s="100" t="s">
-        <v>564</v>
       </c>
     </row>
     <row r="3" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3366,7 +3366,7 @@
         <v>525</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>472</v>
@@ -3487,7 +3487,7 @@
         <v>525</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>476</v>
@@ -3608,7 +3608,7 @@
         <v>525</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E5" s="8" t="s">
         <v>486</v>
@@ -3729,7 +3729,7 @@
         <v>525</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E6" s="8" t="s">
         <v>477</v>
@@ -3850,13 +3850,13 @@
         <v>525</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>543</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>544</v>
+        <v>621</v>
       </c>
       <c r="G7" s="51">
         <v>0</v>
@@ -4002,7 +4002,7 @@
         <v>525</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>129</v>
@@ -4123,7 +4123,7 @@
         <v>525</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>130</v>
@@ -4244,7 +4244,7 @@
         <v>525</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E10" s="75" t="s">
         <v>444</v>
@@ -4365,7 +4365,7 @@
         <v>525</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>114</v>
@@ -4486,7 +4486,7 @@
         <v>525</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>115</v>
@@ -4607,7 +4607,7 @@
         <v>525</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>123</v>
@@ -4728,7 +4728,7 @@
         <v>525</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E14" s="8" t="s">
         <v>113</v>
@@ -4849,7 +4849,7 @@
         <v>525</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>448</v>
@@ -4970,7 +4970,7 @@
         <v>525</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>131</v>
@@ -5091,7 +5091,7 @@
         <v>525</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>116</v>
@@ -5212,7 +5212,7 @@
         <v>525</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>117</v>
@@ -5333,7 +5333,7 @@
         <v>525</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>455</v>
@@ -5454,7 +5454,7 @@
         <v>525</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>462</v>
@@ -5575,7 +5575,7 @@
         <v>525</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>465</v>
@@ -5696,7 +5696,7 @@
         <v>525</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>467</v>
@@ -5817,7 +5817,7 @@
         <v>525</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E23" s="10" t="s">
         <v>133</v>
@@ -5938,7 +5938,7 @@
         <v>525</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E24" s="10" t="s">
         <v>118</v>
@@ -6059,7 +6059,7 @@
         <v>525</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>363</v>
@@ -6180,7 +6180,7 @@
         <v>525</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E26" s="10" t="s">
         <v>365</v>
@@ -6301,7 +6301,7 @@
         <v>525</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E27" s="10" t="s">
         <v>377</v>
@@ -6422,7 +6422,7 @@
         <v>525</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E28" s="10" t="s">
         <v>373</v>
@@ -6543,7 +6543,7 @@
         <v>525</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E29" s="10" t="s">
         <v>372</v>
@@ -6664,7 +6664,7 @@
         <v>525</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>139</v>
@@ -6785,7 +6785,7 @@
         <v>525</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E31" s="10" t="s">
         <v>119</v>
@@ -6906,7 +6906,7 @@
         <v>525</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E32" s="10" t="s">
         <v>134</v>
@@ -7027,7 +7027,7 @@
         <v>525</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E33" s="10" t="s">
         <v>132</v>
@@ -7148,7 +7148,7 @@
         <v>525</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E34" s="10" t="s">
         <v>454</v>
@@ -7269,7 +7269,7 @@
         <v>525</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E35" s="14" t="s">
         <v>137</v>
@@ -7390,7 +7390,7 @@
         <v>525</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E36" s="14" t="s">
         <v>124</v>
@@ -7511,7 +7511,7 @@
         <v>525</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E37" s="14" t="s">
         <v>125</v>
@@ -7632,7 +7632,7 @@
         <v>525</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E38" s="14" t="s">
         <v>126</v>
@@ -7753,7 +7753,7 @@
         <v>525</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E39" s="14" t="s">
         <v>138</v>
@@ -7874,7 +7874,7 @@
         <v>525</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E40" s="14" t="s">
         <v>127</v>
@@ -7995,7 +7995,7 @@
         <v>525</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E41" s="14" t="s">
         <v>128</v>
@@ -8116,7 +8116,7 @@
         <v>525</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E42" s="14" t="s">
         <v>140</v>
@@ -8237,7 +8237,7 @@
         <v>525</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E43" s="14" t="s">
         <v>141</v>
@@ -8358,7 +8358,7 @@
         <v>525</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E44" s="14" t="s">
         <v>142</v>
@@ -8479,7 +8479,7 @@
         <v>525</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E45" s="14" t="s">
         <v>143</v>
@@ -8600,7 +8600,7 @@
         <v>525</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E46" s="14" t="s">
         <v>144</v>
@@ -8721,7 +8721,7 @@
         <v>525</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E47" s="14" t="s">
         <v>145</v>
@@ -8842,7 +8842,7 @@
         <v>525</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E48" s="14" t="s">
         <v>146</v>
@@ -8963,7 +8963,7 @@
         <v>525</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E49" s="14" t="s">
         <v>147</v>
@@ -9084,7 +9084,7 @@
         <v>525</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E50" s="14" t="s">
         <v>435</v>
@@ -9205,7 +9205,7 @@
         <v>525</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E51" s="14" t="s">
         <v>436</v>
@@ -9326,7 +9326,7 @@
         <v>525</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E52" s="14" t="s">
         <v>457</v>
@@ -9447,7 +9447,7 @@
         <v>525</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E53" s="14" t="s">
         <v>135</v>
@@ -9568,7 +9568,7 @@
         <v>525</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E54" s="12" t="s">
         <v>136</v>
@@ -9689,7 +9689,7 @@
         <v>525</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E55" s="12" t="s">
         <v>120</v>
@@ -9810,7 +9810,7 @@
         <v>525</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E56" s="12" t="s">
         <v>121</v>
@@ -9931,7 +9931,7 @@
         <v>525</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E57" s="12" t="s">
         <v>122</v>
@@ -10052,7 +10052,7 @@
         <v>525</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>148</v>
@@ -10173,7 +10173,7 @@
         <v>525</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>380</v>
@@ -10294,7 +10294,7 @@
         <v>525</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>149</v>
@@ -10415,7 +10415,7 @@
         <v>525</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>150</v>
@@ -10536,7 +10536,7 @@
         <v>525</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>151</v>
@@ -10657,7 +10657,7 @@
         <v>525</v>
       </c>
       <c r="D63" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E63" s="18" t="s">
         <v>152</v>
@@ -10778,7 +10778,7 @@
         <v>525</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E64" s="18" t="s">
         <v>284</v>
@@ -10899,7 +10899,7 @@
         <v>525</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E65" s="18" t="s">
         <v>155</v>
@@ -11020,7 +11020,7 @@
         <v>525</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E66" s="18" t="s">
         <v>406</v>
@@ -11141,7 +11141,7 @@
         <v>525</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E67" s="18" t="s">
         <v>153</v>
@@ -11262,7 +11262,7 @@
         <v>525</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E68" s="18" t="s">
         <v>408</v>
@@ -11383,7 +11383,7 @@
         <v>525</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E69" s="18" t="s">
         <v>154</v>
@@ -11504,7 +11504,7 @@
         <v>525</v>
       </c>
       <c r="D70" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E70" s="18" t="s">
         <v>288</v>
@@ -11625,7 +11625,7 @@
         <v>525</v>
       </c>
       <c r="D71" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E71" s="18" t="s">
         <v>381</v>
@@ -11746,7 +11746,7 @@
         <v>525</v>
       </c>
       <c r="D72" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E72" s="18" t="s">
         <v>156</v>
@@ -11867,7 +11867,7 @@
         <v>525</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E73" s="18" t="s">
         <v>157</v>
@@ -11988,7 +11988,7 @@
         <v>525</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E74" s="18" t="s">
         <v>158</v>
@@ -12109,7 +12109,7 @@
         <v>525</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E75" s="18" t="s">
         <v>159</v>
@@ -12230,7 +12230,7 @@
         <v>525</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E76" s="18" t="s">
         <v>160</v>
@@ -12351,7 +12351,7 @@
         <v>525</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E77" s="18" t="s">
         <v>161</v>
@@ -12472,7 +12472,7 @@
         <v>525</v>
       </c>
       <c r="D78" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E78" s="34" t="s">
         <v>418</v>
@@ -12593,7 +12593,7 @@
         <v>525</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E79" s="34" t="s">
         <v>412</v>
@@ -12714,7 +12714,7 @@
         <v>525</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E80" s="34" t="s">
         <v>419</v>
@@ -12835,7 +12835,7 @@
         <v>525</v>
       </c>
       <c r="D81" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E81" s="34" t="s">
         <v>402</v>
@@ -12956,7 +12956,7 @@
         <v>525</v>
       </c>
       <c r="D82" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E82" s="34" t="s">
         <v>415</v>
@@ -13077,7 +13077,7 @@
         <v>525</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E83" s="34" t="s">
         <v>414</v>
@@ -13198,7 +13198,7 @@
         <v>525</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E84" s="34" t="s">
         <v>416</v>
@@ -13319,7 +13319,7 @@
         <v>525</v>
       </c>
       <c r="D85" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E85" s="34" t="s">
         <v>403</v>
@@ -13440,7 +13440,7 @@
         <v>525</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E86" s="34" t="s">
         <v>404</v>
@@ -13561,7 +13561,7 @@
         <v>525</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E87" s="18" t="s">
         <v>162</v>
@@ -13682,7 +13682,7 @@
         <v>525</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E88" s="18" t="s">
         <v>163</v>
@@ -13803,7 +13803,7 @@
         <v>525</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E89" s="18" t="s">
         <v>164</v>
@@ -13924,7 +13924,7 @@
         <v>525</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E90" s="18" t="s">
         <v>165</v>
@@ -14045,7 +14045,7 @@
         <v>525</v>
       </c>
       <c r="D91" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E91" s="18" t="s">
         <v>166</v>
@@ -14166,7 +14166,7 @@
         <v>525</v>
       </c>
       <c r="D92" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E92" s="20" t="s">
         <v>290</v>
@@ -14287,7 +14287,7 @@
         <v>525</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E93" s="20" t="s">
         <v>291</v>
@@ -14408,7 +14408,7 @@
         <v>525</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E94" s="20" t="s">
         <v>295</v>
@@ -14529,7 +14529,7 @@
         <v>525</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E95" s="20" t="s">
         <v>292</v>
@@ -14650,7 +14650,7 @@
         <v>525</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E96" s="20" t="s">
         <v>293</v>
@@ -14771,7 +14771,7 @@
         <v>525</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E97" s="14" t="s">
         <v>171</v>
@@ -14892,7 +14892,7 @@
         <v>525</v>
       </c>
       <c r="D98" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E98" s="14" t="s">
         <v>289</v>
@@ -15013,7 +15013,7 @@
         <v>525</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E99" s="14" t="s">
         <v>170</v>
@@ -15134,7 +15134,7 @@
         <v>525</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E100" s="24" t="s">
         <v>176</v>
@@ -15255,7 +15255,7 @@
         <v>525</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E101" s="24" t="s">
         <v>369</v>
@@ -15376,7 +15376,7 @@
         <v>525</v>
       </c>
       <c r="D102" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E102" s="24" t="s">
         <v>370</v>
@@ -15497,7 +15497,7 @@
         <v>525</v>
       </c>
       <c r="D103" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E103" s="24" t="s">
         <v>371</v>
@@ -15618,7 +15618,7 @@
         <v>525</v>
       </c>
       <c r="D104" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E104" s="24" t="s">
         <v>383</v>
@@ -15739,7 +15739,7 @@
         <v>525</v>
       </c>
       <c r="D105" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E105" s="24" t="s">
         <v>385</v>
@@ -15860,7 +15860,7 @@
         <v>525</v>
       </c>
       <c r="D106" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E106" s="24" t="s">
         <v>503</v>
@@ -16014,7 +16014,7 @@
         <v>525</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E107" s="24" t="s">
         <v>503</v>
@@ -16168,7 +16168,7 @@
         <v>525</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E108" s="24" t="s">
         <v>503</v>
@@ -16322,7 +16322,7 @@
         <v>525</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E109" s="24" t="s">
         <v>503</v>
@@ -16476,7 +16476,7 @@
         <v>525</v>
       </c>
       <c r="D110" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E110" s="24" t="s">
         <v>387</v>
@@ -16597,7 +16597,7 @@
         <v>525</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E111" s="24" t="s">
         <v>389</v>
@@ -16718,7 +16718,7 @@
         <v>525</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E112" s="24" t="s">
         <v>391</v>
@@ -16839,7 +16839,7 @@
         <v>525</v>
       </c>
       <c r="D113" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E113" s="24" t="s">
         <v>393</v>
@@ -16960,7 +16960,7 @@
         <v>525</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E114" s="24" t="s">
         <v>421</v>
@@ -17081,7 +17081,7 @@
         <v>525</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E115" s="24" t="s">
         <v>423</v>
@@ -17235,7 +17235,7 @@
         <v>525</v>
       </c>
       <c r="D116" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E116" s="24" t="s">
         <v>425</v>
@@ -17389,7 +17389,7 @@
         <v>525</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E117" s="24" t="s">
         <v>426</v>
@@ -17510,7 +17510,7 @@
         <v>525</v>
       </c>
       <c r="D118" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E118" s="24" t="s">
         <v>427</v>
@@ -17664,7 +17664,7 @@
         <v>525</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E119" s="24" t="s">
         <v>428</v>
@@ -17818,7 +17818,7 @@
         <v>525</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E120" s="24" t="s">
         <v>395</v>
@@ -17939,7 +17939,7 @@
         <v>525</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E121" s="24" t="s">
         <v>397</v>
@@ -18060,7 +18060,7 @@
         <v>525</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E122" s="14" t="s">
         <v>172</v>
@@ -18181,7 +18181,7 @@
         <v>525</v>
       </c>
       <c r="D123" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E123" s="14" t="s">
         <v>173</v>
@@ -18334,7 +18334,7 @@
         <v>525</v>
       </c>
       <c r="D124" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E124" s="14" t="s">
         <v>174</v>
@@ -18455,7 +18455,7 @@
         <v>525</v>
       </c>
       <c r="D125" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E125" s="14" t="s">
         <v>175</v>
@@ -18576,7 +18576,7 @@
         <v>525</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E126" s="14" t="s">
         <v>450</v>
@@ -18697,7 +18697,7 @@
         <v>525</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E127" s="14" t="s">
         <v>452</v>
@@ -18818,7 +18818,7 @@
         <v>525</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E128" s="69" t="s">
         <v>178</v>
@@ -18937,7 +18937,7 @@
         <v>525</v>
       </c>
       <c r="D129" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E129" s="69" t="s">
         <v>441</v>
@@ -19056,7 +19056,7 @@
         <v>525</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E130" s="69" t="s">
         <v>446</v>
@@ -19177,7 +19177,7 @@
         <v>525</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E131" s="22" t="s">
         <v>177</v>
@@ -19298,7 +19298,7 @@
         <v>525</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E132" s="22" t="s">
         <v>438</v>
@@ -19419,7 +19419,7 @@
         <v>525</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E133" s="22" t="s">
         <v>311</v>
@@ -19540,7 +19540,7 @@
         <v>525</v>
       </c>
       <c r="D134" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E134" s="22" t="s">
         <v>312</v>
@@ -19661,7 +19661,7 @@
         <v>525</v>
       </c>
       <c r="D135" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E135" s="22" t="s">
         <v>313</v>
@@ -19782,7 +19782,7 @@
         <v>525</v>
       </c>
       <c r="D136" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E136" s="22" t="s">
         <v>314</v>
@@ -19903,7 +19903,7 @@
         <v>525</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E137" s="22" t="s">
         <v>178</v>
@@ -20024,7 +20024,7 @@
         <v>525</v>
       </c>
       <c r="D138" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E138" s="22" t="s">
         <v>315</v>
@@ -20145,7 +20145,7 @@
         <v>525</v>
       </c>
       <c r="D139" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E139" s="22" t="s">
         <v>316</v>
@@ -20266,7 +20266,7 @@
         <v>525</v>
       </c>
       <c r="D140" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E140" s="22" t="s">
         <v>317</v>
@@ -20387,7 +20387,7 @@
         <v>525</v>
       </c>
       <c r="D141" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E141" s="22" t="s">
         <v>318</v>
@@ -20508,7 +20508,7 @@
         <v>525</v>
       </c>
       <c r="D142" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E142" s="22" t="s">
         <v>180</v>
@@ -20629,7 +20629,7 @@
         <v>525</v>
       </c>
       <c r="D143" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E143" s="73" t="s">
         <v>181</v>
@@ -20750,7 +20750,7 @@
         <v>525</v>
       </c>
       <c r="D144" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E144" s="24" t="s">
         <v>167</v>
@@ -20871,7 +20871,7 @@
         <v>525</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E145" s="24" t="s">
         <v>168</v>
@@ -20992,7 +20992,7 @@
         <v>525</v>
       </c>
       <c r="D146" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E146" s="24" t="s">
         <v>169</v>
@@ -21113,7 +21113,7 @@
         <v>525</v>
       </c>
       <c r="D147" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E147" s="24" t="s">
         <v>183</v>
@@ -21234,7 +21234,7 @@
         <v>525</v>
       </c>
       <c r="D148" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E148" s="24" t="s">
         <v>303</v>
@@ -21355,7 +21355,7 @@
         <v>525</v>
       </c>
       <c r="D149" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E149" s="24" t="s">
         <v>304</v>
@@ -21476,7 +21476,7 @@
         <v>525</v>
       </c>
       <c r="D150" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E150" s="24" t="s">
         <v>305</v>
@@ -21597,7 +21597,7 @@
         <v>525</v>
       </c>
       <c r="D151" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E151" s="24" t="s">
         <v>306</v>
@@ -21718,7 +21718,7 @@
         <v>525</v>
       </c>
       <c r="D152" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E152" s="24" t="s">
         <v>184</v>
@@ -21839,7 +21839,7 @@
         <v>525</v>
       </c>
       <c r="D153" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E153" s="14" t="s">
         <v>186</v>
@@ -21960,7 +21960,7 @@
         <v>525</v>
       </c>
       <c r="D154" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E154" s="14" t="s">
         <v>307</v>
@@ -22081,7 +22081,7 @@
         <v>525</v>
       </c>
       <c r="D155" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E155" s="14" t="s">
         <v>308</v>
@@ -22202,7 +22202,7 @@
         <v>525</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E156" s="14" t="s">
         <v>309</v>
@@ -22323,7 +22323,7 @@
         <v>525</v>
       </c>
       <c r="D157" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E157" s="14" t="s">
         <v>310</v>
@@ -22444,7 +22444,7 @@
         <v>525</v>
       </c>
       <c r="D158" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E158" s="14" t="s">
         <v>185</v>
@@ -22565,7 +22565,7 @@
         <v>525</v>
       </c>
       <c r="D159" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E159" s="10" t="s">
         <v>187</v>
@@ -22686,7 +22686,7 @@
         <v>525</v>
       </c>
       <c r="D160" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E160" s="10" t="s">
         <v>298</v>
@@ -22807,7 +22807,7 @@
         <v>525</v>
       </c>
       <c r="D161" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E161" s="10" t="s">
         <v>299</v>
@@ -22928,7 +22928,7 @@
         <v>525</v>
       </c>
       <c r="D162" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E162" s="10" t="s">
         <v>300</v>
@@ -23049,7 +23049,7 @@
         <v>525</v>
       </c>
       <c r="D163" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E163" s="10" t="s">
         <v>302</v>
@@ -23170,7 +23170,7 @@
         <v>525</v>
       </c>
       <c r="D164" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E164" s="10" t="s">
         <v>188</v>
@@ -23291,7 +23291,7 @@
         <v>525</v>
       </c>
       <c r="D165" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E165" s="26" t="s">
         <v>189</v>
@@ -23412,7 +23412,7 @@
         <v>525</v>
       </c>
       <c r="D166" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E166" s="26" t="s">
         <v>319</v>
@@ -23533,7 +23533,7 @@
         <v>525</v>
       </c>
       <c r="D167" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E167" s="26" t="s">
         <v>320</v>
@@ -23654,7 +23654,7 @@
         <v>525</v>
       </c>
       <c r="D168" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E168" s="26" t="s">
         <v>321</v>
@@ -23775,7 +23775,7 @@
         <v>525</v>
       </c>
       <c r="D169" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E169" s="26" t="s">
         <v>322</v>
@@ -23896,7 +23896,7 @@
         <v>525</v>
       </c>
       <c r="D170" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E170" s="26" t="s">
         <v>190</v>
@@ -24017,7 +24017,7 @@
         <v>525</v>
       </c>
       <c r="D171" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E171" s="32" t="s">
         <v>191</v>
@@ -24138,7 +24138,7 @@
         <v>525</v>
       </c>
       <c r="D172" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E172" s="32" t="s">
         <v>323</v>
@@ -24259,7 +24259,7 @@
         <v>525</v>
       </c>
       <c r="D173" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E173" s="32" t="s">
         <v>324</v>
@@ -24380,7 +24380,7 @@
         <v>525</v>
       </c>
       <c r="D174" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E174" s="32" t="s">
         <v>325</v>
@@ -24501,7 +24501,7 @@
         <v>525</v>
       </c>
       <c r="D175" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E175" s="32" t="s">
         <v>326</v>
@@ -24622,7 +24622,7 @@
         <v>525</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E176" s="32" t="s">
         <v>192</v>
@@ -24743,7 +24743,7 @@
         <v>525</v>
       </c>
       <c r="D177" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E177" s="12" t="s">
         <v>327</v>
@@ -24864,7 +24864,7 @@
         <v>525</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E178" s="12" t="s">
         <v>329</v>
@@ -24985,7 +24985,7 @@
         <v>525</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E179" s="12" t="s">
         <v>330</v>
@@ -25106,7 +25106,7 @@
         <v>525</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E180" s="12" t="s">
         <v>331</v>
@@ -25227,7 +25227,7 @@
         <v>525</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E181" s="12" t="s">
         <v>332</v>
@@ -25348,7 +25348,7 @@
         <v>525</v>
       </c>
       <c r="D182" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E182" s="12" t="s">
         <v>349</v>
@@ -25469,7 +25469,7 @@
         <v>525</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E183" s="12" t="s">
         <v>350</v>
@@ -25590,7 +25590,7 @@
         <v>525</v>
       </c>
       <c r="D184" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E184" s="28" t="s">
         <v>351</v>
@@ -25711,7 +25711,7 @@
         <v>525</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E185" s="28" t="s">
         <v>333</v>
@@ -25832,7 +25832,7 @@
         <v>525</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E186" s="28" t="s">
         <v>334</v>
@@ -25953,7 +25953,7 @@
         <v>525</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E187" s="28" t="s">
         <v>335</v>
@@ -26074,7 +26074,7 @@
         <v>525</v>
       </c>
       <c r="D188" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E188" s="28" t="s">
         <v>336</v>
@@ -26195,7 +26195,7 @@
         <v>525</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E189" s="28" t="s">
         <v>353</v>
@@ -26316,7 +26316,7 @@
         <v>525</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E190" s="24" t="s">
         <v>193</v>
@@ -26437,7 +26437,7 @@
         <v>525</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E191" s="24" t="s">
         <v>337</v>
@@ -26558,7 +26558,7 @@
         <v>525</v>
       </c>
       <c r="D192" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E192" s="24" t="s">
         <v>338</v>
@@ -26679,7 +26679,7 @@
         <v>525</v>
       </c>
       <c r="D193" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E193" s="24" t="s">
         <v>339</v>
@@ -26800,7 +26800,7 @@
         <v>525</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E194" s="24" t="s">
         <v>340</v>
@@ -26921,7 +26921,7 @@
         <v>525</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E195" s="24" t="s">
         <v>194</v>
@@ -27042,7 +27042,7 @@
         <v>525</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E196" s="8" t="s">
         <v>355</v>
@@ -27163,7 +27163,7 @@
         <v>525</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E197" s="8" t="s">
         <v>341</v>
@@ -27284,7 +27284,7 @@
         <v>525</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E198" s="8" t="s">
         <v>342</v>
@@ -27405,7 +27405,7 @@
         <v>525</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E199" s="8" t="s">
         <v>343</v>
@@ -27526,7 +27526,7 @@
         <v>525</v>
       </c>
       <c r="D200" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E200" s="8" t="s">
         <v>344</v>
@@ -27647,7 +27647,7 @@
         <v>525</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E201" s="8" t="s">
         <v>358</v>
@@ -27768,7 +27768,7 @@
         <v>525</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E202" s="30" t="s">
         <v>356</v>
@@ -27889,7 +27889,7 @@
         <v>525</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E203" s="30" t="s">
         <v>345</v>
@@ -28010,7 +28010,7 @@
         <v>525</v>
       </c>
       <c r="D204" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E204" s="30" t="s">
         <v>346</v>
@@ -28131,7 +28131,7 @@
         <v>525</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E205" s="30" t="s">
         <v>347</v>
@@ -28252,7 +28252,7 @@
         <v>525</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E206" s="30" t="s">
         <v>348</v>
@@ -28373,7 +28373,7 @@
         <v>525</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E207" s="30" t="s">
         <v>360</v>
@@ -28494,7 +28494,7 @@
         <v>525</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E208" s="93" t="s">
         <v>203</v>
@@ -28606,7 +28606,7 @@
     </row>
     <row r="209" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
       <c r="B209" s="3" t="s">
         <v>470</v>
@@ -28615,7 +28615,7 @@
         <v>525</v>
       </c>
       <c r="D209" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E209" s="30" t="s">
         <v>491</v>
@@ -28754,7 +28754,7 @@
     </row>
     <row r="210" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
       <c r="B210" s="3" t="s">
         <v>470</v>
@@ -28763,7 +28763,7 @@
         <v>525</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E210" s="30" t="s">
         <v>493</v>
@@ -28884,7 +28884,7 @@
         <v>525</v>
       </c>
       <c r="D211" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E211" s="30" t="s">
         <v>514</v>
@@ -28996,7 +28996,7 @@
     </row>
     <row r="212" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
       <c r="B212" s="3" t="s">
         <v>470</v>
@@ -29005,7 +29005,7 @@
         <v>525</v>
       </c>
       <c r="D212" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E212" s="96" t="s">
         <v>509</v>
@@ -29146,7 +29146,7 @@
         <v>525</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E213" s="96" t="s">
         <v>510</v>
@@ -29267,7 +29267,7 @@
         <v>525</v>
       </c>
       <c r="D214" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E214" s="96" t="s">
         <v>511</v>
@@ -29388,7 +29388,7 @@
         <v>525</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E215" s="96" t="s">
         <v>512</v>
@@ -29509,7 +29509,7 @@
         <v>525</v>
       </c>
       <c r="D216" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E216" s="96" t="s">
         <v>516</v>
@@ -29630,7 +29630,7 @@
         <v>525</v>
       </c>
       <c r="D217" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E217" s="96" t="s">
         <v>518</v>
@@ -29784,7 +29784,7 @@
         <v>525</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E218" s="96" t="s">
         <v>523</v>
@@ -29896,7 +29896,7 @@
     </row>
     <row r="219" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
       <c r="B219" s="3" t="s">
         <v>470</v>
@@ -29905,13 +29905,13 @@
         <v>525</v>
       </c>
       <c r="D219" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E219" s="96" t="s">
+        <v>551</v>
+      </c>
+      <c r="F219" s="96" t="s">
         <v>552</v>
-      </c>
-      <c r="F219" s="96" t="s">
-        <v>553</v>
       </c>
       <c r="G219" s="98">
         <v>2.4999999999999998E-12</v>
@@ -30017,7 +30017,7 @@
     </row>
     <row r="220" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
       <c r="B220" s="3" t="s">
         <v>470</v>
@@ -30026,13 +30026,13 @@
         <v>525</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E220" s="96" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
       <c r="F220" s="96" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
       <c r="G220" s="98">
         <v>1.2E-8</v>
@@ -30158,7 +30158,7 @@
     </row>
     <row r="221" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="B221" s="3" t="s">
         <v>470</v>
@@ -30167,13 +30167,13 @@
         <v>525</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E221" s="96" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="F221" s="96" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="G221" s="98">
         <v>9.9999999999999995E-8</v>
@@ -30279,7 +30279,7 @@
     </row>
     <row r="222" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="B222" s="3" t="s">
         <v>470</v>
@@ -30288,13 +30288,13 @@
         <v>525</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E222" s="96" t="s">
+        <v>556</v>
+      </c>
+      <c r="F222" s="96" t="s">
         <v>557</v>
-      </c>
-      <c r="F222" s="96" t="s">
-        <v>558</v>
       </c>
       <c r="G222" s="98">
         <f>2*0.00001</f>
@@ -30411,10 +30411,10 @@
         <v>525</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E223" s="96" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="F223" s="96" t="s">
         <v>521</v>
@@ -30556,7 +30556,7 @@
     </row>
     <row r="224" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="B224" s="3" t="s">
         <v>470</v>
@@ -30565,13 +30565,13 @@
         <v>525</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E224" s="96" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="F224" s="96" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="G224" s="98">
         <f>0.00000000000001 * 10000</f>
@@ -30710,7 +30710,7 @@
     </row>
     <row r="225" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="B225" s="3" t="s">
         <v>470</v>
@@ -30719,10 +30719,10 @@
         <v>525</v>
       </c>
       <c r="D225" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E225" s="96" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="F225" s="96" t="s">
         <v>504</v>
@@ -30833,7 +30833,7 @@
     </row>
     <row r="226" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B226" s="3" t="s">
         <v>470</v>
@@ -30842,10 +30842,10 @@
         <v>525</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E226" s="96" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
       <c r="F226" s="96" t="s">
         <v>490</v>
@@ -30954,7 +30954,7 @@
     </row>
     <row r="227" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B227" s="3" t="s">
         <v>470</v>
@@ -30963,10 +30963,10 @@
         <v>525</v>
       </c>
       <c r="D227" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E227" s="96" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
       <c r="F227" s="96" t="s">
         <v>508</v>
@@ -31075,7 +31075,7 @@
     </row>
     <row r="228" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
       <c r="B228" s="3" t="s">
         <v>470</v>
@@ -31084,10 +31084,10 @@
         <v>525</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E228" s="96" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
       <c r="F228" s="96" t="s">
         <v>508</v>
@@ -31229,7 +31229,7 @@
     </row>
     <row r="229" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
       <c r="B229" s="3" t="s">
         <v>470</v>
@@ -31238,10 +31238,10 @@
         <v>525</v>
       </c>
       <c r="D229" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E229" s="96" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
       <c r="F229" s="96" t="s">
         <v>508</v>
@@ -31350,7 +31350,7 @@
     </row>
     <row r="230" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
       <c r="B230" s="3" t="s">
         <v>470</v>
@@ -31359,10 +31359,10 @@
         <v>525</v>
       </c>
       <c r="D230" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="E230" s="96" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
       <c r="F230" s="96" t="s">
         <v>508</v>
@@ -31764,7 +31764,7 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="35.7109375" customWidth="1"/>
     <col min="3" max="3" width="49.5703125" customWidth="1"/>

</xml_diff>

<commit_message>
solved young equation derivation to apply solver and gain more stability in water model
</commit_message>
<xml_diff>
--- a/simulations/inputs/Scenarios_24_09_22.xlsx
+++ b/simulations/inputs/Scenarios_24_09_22.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tigerault\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\sshfs\torisuten@192.168.12.9\package\Wheat-BRIDGES\Root_BRIDGES\root_cynaps\simulations\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B483C5F9-30DC-4194-A959-461CE8572CD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFF84910-86BA-44D3-8FB4-6CCCEC2F9A6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28785" yWindow="-21435" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="scenarios_as_columns" sheetId="2" r:id="rId1"/>
@@ -2773,48 +2773,48 @@
     </xf>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
     <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Avertissement" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Calcul" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Cellule liée" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Entrée" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Insatisfaisant" xfId="7" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Neutre" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Satisfaisant" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Sortie" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texte explicatif" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Titre" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Titre 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Titre 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Titre 3" xfId="4" builtinId="18" customBuiltin="1"/>
-    <cellStyle name="Titre 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
-    <cellStyle name="Vérification" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3095,25 +3095,25 @@
   <dimension ref="A1:AO230"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="7" ySplit="1" topLeftCell="H189" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="7" ySplit="1" topLeftCell="J157" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="H1" sqref="H1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J209" sqref="J209:J210"/>
+      <selection pane="bottomRight" activeCell="L225" sqref="L225"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32.6640625" style="1" customWidth="1"/>
     <col min="2" max="4" width="15" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.5703125" style="37" customWidth="1"/>
-    <col min="8" max="8" width="39.85546875" style="1" customWidth="1"/>
-    <col min="9" max="9" width="10.42578125" style="1" customWidth="1"/>
-    <col min="10" max="41" width="39.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.5546875" style="37" customWidth="1"/>
+    <col min="8" max="8" width="39.88671875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="10.44140625" style="1" customWidth="1"/>
+    <col min="10" max="41" width="39.88671875" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>468</v>
       </c>
@@ -3234,7 +3234,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="2" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="74" t="s">
         <v>526</v>
       </c>
@@ -3355,7 +3355,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="3" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>481</v>
       </c>
@@ -3476,7 +3476,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="4" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>480</v>
       </c>
@@ -3597,7 +3597,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="5" spans="1:41" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" s="1" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>485</v>
       </c>
@@ -3718,7 +3718,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="6" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>482</v>
       </c>
@@ -3839,7 +3839,7 @@
         <v>489</v>
       </c>
     </row>
-    <row r="7" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>542</v>
       </c>
@@ -3991,7 +3991,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>2</v>
       </c>
@@ -4112,7 +4112,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>3</v>
       </c>
@@ -4233,7 +4233,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A10" s="74" t="s">
         <v>443</v>
       </c>
@@ -4354,7 +4354,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>4</v>
       </c>
@@ -4475,7 +4475,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>5</v>
       </c>
@@ -4596,7 +4596,7 @@
         <v>4.1666666999999998E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -4717,7 +4717,7 @@
         <v>4.1666666999999998E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A14" s="7" t="s">
         <v>1</v>
       </c>
@@ -4838,7 +4838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
         <v>447</v>
       </c>
@@ -4959,7 +4959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A16" s="7" t="s">
         <v>6</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A17" s="7" t="s">
         <v>7</v>
       </c>
@@ -5201,7 +5201,7 @@
         <v>5.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
         <v>8</v>
       </c>
@@ -5322,7 +5322,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A19" s="7" t="s">
         <v>460</v>
       </c>
@@ -5443,7 +5443,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
         <v>461</v>
       </c>
@@ -5564,7 +5564,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A21" s="7" t="s">
         <v>464</v>
       </c>
@@ -5685,7 +5685,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A22" s="7" t="s">
         <v>466</v>
       </c>
@@ -5806,7 +5806,7 @@
         <v>86400</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
         <v>10</v>
       </c>
@@ -5927,7 +5927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
         <v>11</v>
       </c>
@@ -6048,7 +6048,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
         <v>362</v>
       </c>
@@ -6169,7 +6169,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
         <v>364</v>
       </c>
@@ -6290,7 +6290,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
         <v>376</v>
       </c>
@@ -6411,7 +6411,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
         <v>375</v>
       </c>
@@ -6532,7 +6532,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
         <v>374</v>
       </c>
@@ -6653,7 +6653,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A30" s="9" t="s">
         <v>12</v>
       </c>
@@ -6774,7 +6774,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A31" s="9" t="s">
         <v>13</v>
       </c>
@@ -6895,7 +6895,7 @@
         <v>0.33</v>
       </c>
     </row>
-    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A32" s="9" t="s">
         <v>14</v>
       </c>
@@ -7016,7 +7016,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A33" s="9" t="s">
         <v>9</v>
       </c>
@@ -7137,7 +7137,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A34" s="9" t="s">
         <v>453</v>
       </c>
@@ -7258,7 +7258,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A35" s="13" t="s">
         <v>21</v>
       </c>
@@ -7379,7 +7379,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A36" s="13" t="s">
         <v>22</v>
       </c>
@@ -7500,7 +7500,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A37" s="13" t="s">
         <v>23</v>
       </c>
@@ -7621,7 +7621,7 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A38" s="13" t="s">
         <v>24</v>
       </c>
@@ -7742,7 +7742,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A39" s="13" t="s">
         <v>25</v>
       </c>
@@ -7863,7 +7863,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A40" s="13" t="s">
         <v>26</v>
       </c>
@@ -7984,7 +7984,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A41" s="13" t="s">
         <v>27</v>
       </c>
@@ -8105,7 +8105,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A42" s="13" t="s">
         <v>28</v>
       </c>
@@ -8226,7 +8226,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>29</v>
       </c>
@@ -8347,7 +8347,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A44" s="13" t="s">
         <v>30</v>
       </c>
@@ -8468,7 +8468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A45" s="13" t="s">
         <v>31</v>
       </c>
@@ -8589,7 +8589,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A46" s="13" t="s">
         <v>32</v>
       </c>
@@ -8710,7 +8710,7 @@
         <v>-0.1</v>
       </c>
     </row>
-    <row r="47" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>33</v>
       </c>
@@ -8831,7 +8831,7 @@
         <v>-0.2</v>
       </c>
     </row>
-    <row r="48" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A48" s="13" t="s">
         <v>34</v>
       </c>
@@ -8952,7 +8952,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="49" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A49" s="13" t="s">
         <v>35</v>
       </c>
@@ -9073,7 +9073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A50" s="13" t="s">
         <v>433</v>
       </c>
@@ -9194,7 +9194,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="51" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A51" s="13" t="s">
         <v>434</v>
       </c>
@@ -9315,7 +9315,7 @@
         <v>1200</v>
       </c>
     </row>
-    <row r="52" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A52" s="13" t="s">
         <v>456</v>
       </c>
@@ -9436,7 +9436,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="53" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A53" s="13" t="s">
         <v>15</v>
       </c>
@@ -9557,7 +9557,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="54" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A54" s="11" t="s">
         <v>16</v>
       </c>
@@ -9678,7 +9678,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="55" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
         <v>17</v>
       </c>
@@ -9799,7 +9799,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A56" s="11" t="s">
         <v>18</v>
       </c>
@@ -9920,7 +9920,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="57" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A57" s="11" t="s">
         <v>19</v>
       </c>
@@ -10041,7 +10041,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="58" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>36</v>
       </c>
@@ -10162,7 +10162,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A59" s="15" t="s">
         <v>379</v>
       </c>
@@ -10283,7 +10283,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A60" s="15" t="s">
         <v>37</v>
       </c>
@@ -10404,7 +10404,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="61" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A61" s="15" t="s">
         <v>38</v>
       </c>
@@ -10525,7 +10525,7 @@
         <v>1E-4</v>
       </c>
     </row>
-    <row r="62" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A62" s="17" t="s">
         <v>39</v>
       </c>
@@ -10646,7 +10646,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
     </row>
-    <row r="63" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A63" s="17" t="s">
         <v>40</v>
       </c>
@@ -10767,7 +10767,7 @@
         <v>1.22E-4</v>
       </c>
     </row>
-    <row r="64" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A64" s="17" t="s">
         <v>206</v>
       </c>
@@ -10888,7 +10888,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A65" s="17" t="s">
         <v>41</v>
       </c>
@@ -11009,7 +11009,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="66" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A66" s="17" t="s">
         <v>405</v>
       </c>
@@ -11130,7 +11130,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="67" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A67" s="17" t="s">
         <v>90</v>
       </c>
@@ -11251,7 +11251,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A68" s="17" t="s">
         <v>407</v>
       </c>
@@ -11372,7 +11372,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="69" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A69" s="17" t="s">
         <v>42</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="70" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A70" s="17" t="s">
         <v>207</v>
       </c>
@@ -11614,7 +11614,7 @@
         <v>1453890.8941884842</v>
       </c>
     </row>
-    <row r="71" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A71" s="17" t="s">
         <v>43</v>
       </c>
@@ -11735,7 +11735,7 @@
         <v>1.3888888888888888E-5</v>
       </c>
     </row>
-    <row r="72" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A72" s="17" t="s">
         <v>44</v>
       </c>
@@ -11856,7 +11856,7 @@
         <v>6.5011574074074071E-4</v>
       </c>
     </row>
-    <row r="73" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A73" s="17" t="s">
         <v>45</v>
       </c>
@@ -11977,7 +11977,7 @@
         <v>4.7400000000000003E-3</v>
       </c>
     </row>
-    <row r="74" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A74" s="17" t="s">
         <v>46</v>
       </c>
@@ -12098,7 +12098,7 @@
         <v>282528</v>
       </c>
     </row>
-    <row r="75" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A75" s="17" t="s">
         <v>47</v>
       </c>
@@ -12219,7 +12219,7 @@
         <v>0.56999999999999995</v>
       </c>
     </row>
-    <row r="76" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A76" s="17" t="s">
         <v>48</v>
       </c>
@@ -12340,7 +12340,7 @@
         <v>0.16</v>
       </c>
     </row>
-    <row r="77" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A77" s="17" t="s">
         <v>49</v>
       </c>
@@ -12461,7 +12461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A78" s="33" t="s">
         <v>50</v>
       </c>
@@ -12582,7 +12582,7 @@
         <v>745476480000</v>
       </c>
     </row>
-    <row r="79" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A79" s="33" t="s">
         <v>204</v>
       </c>
@@ -12703,7 +12703,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A80" s="33" t="s">
         <v>413</v>
       </c>
@@ -12824,7 +12824,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="81" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A81" s="33" t="s">
         <v>399</v>
       </c>
@@ -12945,7 +12945,7 @@
         <v>21600</v>
       </c>
     </row>
-    <row r="82" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A82" s="33" t="s">
         <v>409</v>
       </c>
@@ -13066,7 +13066,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="83" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A83" s="33" t="s">
         <v>400</v>
       </c>
@@ -13187,7 +13187,7 @@
         <v>60479.999999999993</v>
       </c>
     </row>
-    <row r="84" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A84" s="33" t="s">
         <v>410</v>
       </c>
@@ -13308,7 +13308,7 @@
         <v>0.85</v>
       </c>
     </row>
-    <row r="85" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A85" s="33" t="s">
         <v>401</v>
       </c>
@@ -13429,7 +13429,7 @@
         <v>518400</v>
       </c>
     </row>
-    <row r="86" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A86" s="33" t="s">
         <v>411</v>
       </c>
@@ -13550,7 +13550,7 @@
         <v>5184000</v>
       </c>
     </row>
-    <row r="87" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A87" s="17" t="s">
         <v>51</v>
       </c>
@@ -13671,7 +13671,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="88" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A88" s="17" t="s">
         <v>52</v>
       </c>
@@ -13792,7 +13792,7 @@
         <v>140000</v>
       </c>
     </row>
-    <row r="89" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A89" s="17" t="s">
         <v>53</v>
       </c>
@@ -13913,7 +13913,7 @@
         <v>3.6636136999999999E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A90" s="17" t="s">
         <v>54</v>
       </c>
@@ -14034,7 +14034,7 @@
         <v>4.4999999999999997E-3</v>
       </c>
     </row>
-    <row r="91" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A91" s="17" t="s">
         <v>55</v>
       </c>
@@ -14155,7 +14155,7 @@
         <v>0.06</v>
       </c>
     </row>
-    <row r="92" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A92" s="19" t="s">
         <v>213</v>
       </c>
@@ -14276,7 +14276,7 @@
         <v>6.0000000000000002E-6</v>
       </c>
     </row>
-    <row r="93" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A93" s="19" t="s">
         <v>214</v>
       </c>
@@ -14397,7 +14397,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="94" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A94" s="19" t="s">
         <v>215</v>
       </c>
@@ -14518,7 +14518,7 @@
         <v>374999999.99999994</v>
       </c>
     </row>
-    <row r="95" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A95" s="19" t="s">
         <v>216</v>
       </c>
@@ -14639,7 +14639,7 @@
         <v>3.7037037037037038E-3</v>
       </c>
     </row>
-    <row r="96" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A96" s="19" t="s">
         <v>217</v>
       </c>
@@ -14760,7 +14760,7 @@
         <v>165600</v>
       </c>
     </row>
-    <row r="97" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A97" s="13" t="s">
         <v>60</v>
       </c>
@@ -14881,7 +14881,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="98" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A98" s="13" t="s">
         <v>208</v>
       </c>
@@ -15002,7 +15002,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="99" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A99" s="13" t="s">
         <v>59</v>
       </c>
@@ -15123,7 +15123,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="100" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A100" s="23" t="s">
         <v>65</v>
       </c>
@@ -15244,7 +15244,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="101" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A101" s="23" t="s">
         <v>366</v>
       </c>
@@ -15365,7 +15365,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="102" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A102" s="23" t="s">
         <v>367</v>
       </c>
@@ -15486,7 +15486,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="103" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A103" s="23" t="s">
         <v>368</v>
       </c>
@@ -15607,7 +15607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="104" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A104" s="23" t="s">
         <v>498</v>
       </c>
@@ -15728,7 +15728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A105" s="23" t="s">
         <v>384</v>
       </c>
@@ -15849,7 +15849,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="106" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A106" s="23" t="s">
         <v>499</v>
       </c>
@@ -16003,7 +16003,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="107" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A107" s="23" t="s">
         <v>500</v>
       </c>
@@ -16157,7 +16157,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="108" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A108" s="23" t="s">
         <v>501</v>
       </c>
@@ -16311,7 +16311,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="109" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A109" s="23" t="s">
         <v>502</v>
       </c>
@@ -16465,7 +16465,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="110" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A110" s="23" t="s">
         <v>386</v>
       </c>
@@ -16586,7 +16586,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A111" s="23" t="s">
         <v>388</v>
       </c>
@@ -16707,7 +16707,7 @@
         <v>1589759.9999999998</v>
       </c>
     </row>
-    <row r="112" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A112" s="23" t="s">
         <v>390</v>
       </c>
@@ -16828,7 +16828,7 @@
         <v>6171428.5714285718</v>
       </c>
     </row>
-    <row r="113" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A113" s="23" t="s">
         <v>392</v>
       </c>
@@ -16949,7 +16949,7 @@
         <v>6171428.5714285718</v>
       </c>
     </row>
-    <row r="114" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A114" s="23" t="s">
         <v>420</v>
       </c>
@@ -17070,7 +17070,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="115" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="23" t="s">
         <v>422</v>
       </c>
@@ -17224,7 +17224,7 @@
         <v>28080</v>
       </c>
     </row>
-    <row r="116" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A116" s="23" t="s">
         <v>424</v>
       </c>
@@ -17378,7 +17378,7 @@
         <v>0.11100000000000002</v>
       </c>
     </row>
-    <row r="117" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A117" s="23" t="s">
         <v>495</v>
       </c>
@@ -17499,7 +17499,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="118" spans="1:41" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:41" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="23" t="s">
         <v>496</v>
       </c>
@@ -17653,7 +17653,7 @@
         <v>459648</v>
       </c>
     </row>
-    <row r="119" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A119" s="23" t="s">
         <v>497</v>
       </c>
@@ -17807,7 +17807,7 @@
         <v>0.13875000000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A120" s="23" t="s">
         <v>394</v>
       </c>
@@ -17928,7 +17928,7 @@
         <v>21600</v>
       </c>
     </row>
-    <row r="121" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A121" s="23" t="s">
         <v>396</v>
       </c>
@@ -18049,7 +18049,7 @@
         <v>43200</v>
       </c>
     </row>
-    <row r="122" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A122" s="13" t="s">
         <v>61</v>
       </c>
@@ -18170,7 +18170,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="123" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A123" s="13" t="s">
         <v>62</v>
       </c>
@@ -18323,7 +18323,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="124" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A124" s="13" t="s">
         <v>63</v>
       </c>
@@ -18444,7 +18444,7 @@
         <v>5.7899999999999998E-7</v>
       </c>
     </row>
-    <row r="125" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A125" s="13" t="s">
         <v>64</v>
       </c>
@@ -18565,7 +18565,7 @@
         <v>2.0833333333333335E-4</v>
       </c>
     </row>
-    <row r="126" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A126" s="13" t="s">
         <v>449</v>
       </c>
@@ -18686,7 +18686,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A127" s="13" t="s">
         <v>451</v>
       </c>
@@ -18807,7 +18807,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A128" s="68" t="s">
         <v>440</v>
       </c>
@@ -18926,7 +18926,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A129" s="68" t="s">
         <v>67</v>
       </c>
@@ -19045,7 +19045,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A130" s="68" t="s">
         <v>445</v>
       </c>
@@ -19166,7 +19166,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="131" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A131" s="21" t="s">
         <v>66</v>
       </c>
@@ -19287,7 +19287,7 @@
         <v>5.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="132" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A132" s="21" t="s">
         <v>437</v>
       </c>
@@ -19408,7 +19408,7 @@
         <v>4.9999999999999999E-13</v>
       </c>
     </row>
-    <row r="133" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A133" s="21" t="s">
         <v>228</v>
       </c>
@@ -19529,7 +19529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="134" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A134" s="21" t="s">
         <v>229</v>
       </c>
@@ -19650,7 +19650,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="135" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A135" s="21" t="s">
         <v>230</v>
       </c>
@@ -19771,7 +19771,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="136" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A136" s="21" t="s">
         <v>231</v>
       </c>
@@ -19892,7 +19892,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="137" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A137" s="21" t="s">
         <v>68</v>
       </c>
@@ -20013,7 +20013,7 @@
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="138" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A138" s="21" t="s">
         <v>232</v>
       </c>
@@ -20134,7 +20134,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="139" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A139" s="21" t="s">
         <v>233</v>
       </c>
@@ -20255,7 +20255,7 @@
         <v>-0.04</v>
       </c>
     </row>
-    <row r="140" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A140" s="21" t="s">
         <v>234</v>
       </c>
@@ -20376,7 +20376,7 @@
         <v>2.9</v>
       </c>
     </row>
-    <row r="141" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A141" s="21" t="s">
         <v>235</v>
       </c>
@@ -20497,7 +20497,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A142" s="21" t="s">
         <v>69</v>
       </c>
@@ -20618,7 +20618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A143" s="72" t="s">
         <v>70</v>
       </c>
@@ -20739,7 +20739,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
-    <row r="144" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A144" s="23" t="s">
         <v>56</v>
       </c>
@@ -20860,7 +20860,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A145" s="23" t="s">
         <v>57</v>
       </c>
@@ -20981,7 +20981,7 @@
         <v>2E-3</v>
       </c>
     </row>
-    <row r="146" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A146" s="23" t="s">
         <v>58</v>
       </c>
@@ -21102,7 +21102,7 @@
         <v>3.9999999999999998E-6</v>
       </c>
     </row>
-    <row r="147" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A147" s="23" t="s">
         <v>71</v>
       </c>
@@ -21223,7 +21223,7 @@
         <v>3.7699999999999999E-10</v>
       </c>
     </row>
-    <row r="148" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A148" s="23" t="s">
         <v>236</v>
       </c>
@@ -21344,7 +21344,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="149" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A149" s="23" t="s">
         <v>237</v>
       </c>
@@ -21465,7 +21465,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="150" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A150" s="23" t="s">
         <v>238</v>
       </c>
@@ -21586,7 +21586,7 @@
         <v>0.89100000000000001</v>
       </c>
     </row>
-    <row r="151" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A151" s="23" t="s">
         <v>239</v>
       </c>
@@ -21707,7 +21707,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A152" s="23" t="s">
         <v>72</v>
       </c>
@@ -21828,7 +21828,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="153" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A153" s="13" t="s">
         <v>73</v>
       </c>
@@ -21949,7 +21949,7 @@
         <v>5.8333333333333335E-9</v>
       </c>
     </row>
-    <row r="154" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A154" s="13" t="s">
         <v>240</v>
       </c>
@@ -22070,7 +22070,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="155" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A155" s="13" t="s">
         <v>241</v>
       </c>
@@ -22191,7 +22191,7 @@
         <v>-0.06</v>
       </c>
     </row>
-    <row r="156" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A156" s="13" t="s">
         <v>242</v>
       </c>
@@ -22312,7 +22312,7 @@
         <v>0.89100000000000001</v>
       </c>
     </row>
-    <row r="157" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A157" s="13" t="s">
         <v>243</v>
       </c>
@@ -22433,7 +22433,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A158" s="13" t="s">
         <v>74</v>
       </c>
@@ -22554,7 +22554,7 @@
         <v>4.0000000000000003E-5</v>
       </c>
     </row>
-    <row r="159" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A159" s="9" t="s">
         <v>75</v>
       </c>
@@ -22675,7 +22675,7 @@
         <v>4.0000000000000001E-8</v>
       </c>
     </row>
-    <row r="160" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A160" s="9" t="s">
         <v>218</v>
       </c>
@@ -22796,7 +22796,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="161" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A161" s="9" t="s">
         <v>219</v>
       </c>
@@ -22917,7 +22917,7 @@
         <v>-4.4200000000000003E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A162" s="9" t="s">
         <v>220</v>
       </c>
@@ -23038,7 +23038,7 @@
         <v>1.55</v>
       </c>
     </row>
-    <row r="163" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A163" s="9" t="s">
         <v>221</v>
       </c>
@@ -23159,7 +23159,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="164" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A164" s="9" t="s">
         <v>76</v>
       </c>
@@ -23280,7 +23280,7 @@
         <v>2.7799999999999998E-4</v>
       </c>
     </row>
-    <row r="165" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A165" s="25" t="s">
         <v>78</v>
       </c>
@@ -23401,7 +23401,7 @@
         <v>2.4999999999999998E-12</v>
       </c>
     </row>
-    <row r="166" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A166" s="25" t="s">
         <v>245</v>
       </c>
@@ -23522,7 +23522,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A167" s="25" t="s">
         <v>246</v>
       </c>
@@ -23643,7 +23643,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A168" s="25" t="s">
         <v>247</v>
       </c>
@@ -23764,7 +23764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="169" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A169" s="25" t="s">
         <v>248</v>
       </c>
@@ -23885,7 +23885,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A170" s="25" t="s">
         <v>79</v>
       </c>
@@ -24006,7 +24006,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="171" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A171" s="31" t="s">
         <v>80</v>
       </c>
@@ -24127,7 +24127,7 @@
         <v>2.0000000000000001E-9</v>
       </c>
     </row>
-    <row r="172" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A172" s="31" t="s">
         <v>249</v>
       </c>
@@ -24248,7 +24248,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="173" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A173" s="31" t="s">
         <v>250</v>
       </c>
@@ -24369,7 +24369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A174" s="31" t="s">
         <v>251</v>
       </c>
@@ -24490,7 +24490,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="175" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A175" s="31" t="s">
         <v>252</v>
       </c>
@@ -24611,7 +24611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="176" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A176" s="31" t="s">
         <v>81</v>
       </c>
@@ -24732,7 +24732,7 @@
         <v>1.6666666666666666E-4</v>
       </c>
     </row>
-    <row r="177" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A177" s="11" t="s">
         <v>253</v>
       </c>
@@ -24853,7 +24853,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="178" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A178" s="11" t="s">
         <v>254</v>
       </c>
@@ -24974,7 +24974,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="179" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A179" s="11" t="s">
         <v>255</v>
       </c>
@@ -25095,7 +25095,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A180" s="11" t="s">
         <v>256</v>
       </c>
@@ -25216,7 +25216,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="181" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A181" s="11" t="s">
         <v>257</v>
       </c>
@@ -25337,7 +25337,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A182" s="11" t="s">
         <v>258</v>
       </c>
@@ -25458,7 +25458,7 @@
         <v>8.3333333333333331E-5</v>
       </c>
     </row>
-    <row r="183" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A183" s="11" t="s">
         <v>259</v>
       </c>
@@ -25579,7 +25579,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="184" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A184" s="27" t="s">
         <v>260</v>
       </c>
@@ -25700,7 +25700,7 @@
         <v>2.3533050791148899E-8</v>
       </c>
     </row>
-    <row r="185" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A185" s="27" t="s">
         <v>261</v>
       </c>
@@ -25821,7 +25821,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="186" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A186" s="27" t="s">
         <v>262</v>
       </c>
@@ -25942,7 +25942,7 @@
         <v>-0.187</v>
       </c>
     </row>
-    <row r="187" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A187" s="27" t="s">
         <v>263</v>
       </c>
@@ -26063,7 +26063,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="188" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A188" s="27" t="s">
         <v>264</v>
       </c>
@@ -26184,7 +26184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="189" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A189" s="27" t="s">
         <v>265</v>
       </c>
@@ -26305,7 +26305,7 @@
         <v>6.1060227588121015E-4</v>
       </c>
     </row>
-    <row r="190" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A190" s="23" t="s">
         <v>266</v>
       </c>
@@ -26426,7 +26426,7 @@
         <v>3.9999999999999998E-7</v>
       </c>
     </row>
-    <row r="191" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A191" s="23" t="s">
         <v>267</v>
       </c>
@@ -26547,7 +26547,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="192" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A192" s="23" t="s">
         <v>268</v>
       </c>
@@ -26668,7 +26668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A193" s="23" t="s">
         <v>269</v>
       </c>
@@ -26789,7 +26789,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="194" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A194" s="23" t="s">
         <v>270</v>
       </c>
@@ -26910,7 +26910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="195" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A195" s="23" t="s">
         <v>271</v>
       </c>
@@ -27031,7 +27031,7 @@
         <v>8.3333333333333331E-5</v>
       </c>
     </row>
-    <row r="196" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A196" s="7" t="s">
         <v>272</v>
       </c>
@@ -27152,7 +27152,7 @@
         <v>3.9999999999999998E-7</v>
       </c>
     </row>
-    <row r="197" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A197" s="7" t="s">
         <v>273</v>
       </c>
@@ -27273,7 +27273,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="198" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A198" s="7" t="s">
         <v>274</v>
       </c>
@@ -27394,7 +27394,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A199" s="7" t="s">
         <v>275</v>
       </c>
@@ -27515,7 +27515,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="200" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A200" s="7" t="s">
         <v>276</v>
       </c>
@@ -27636,7 +27636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="201" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A201" s="7" t="s">
         <v>277</v>
       </c>
@@ -27757,7 +27757,7 @@
         <v>8.3333333333333331E-5</v>
       </c>
     </row>
-    <row r="202" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A202" s="29" t="s">
         <v>278</v>
       </c>
@@ -27878,7 +27878,7 @@
         <v>1.9999999999999999E-7</v>
       </c>
     </row>
-    <row r="203" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A203" s="29" t="s">
         <v>279</v>
       </c>
@@ -27999,7 +27999,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="204" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A204" s="29" t="s">
         <v>280</v>
       </c>
@@ -28120,7 +28120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A205" s="29" t="s">
         <v>281</v>
       </c>
@@ -28241,7 +28241,7 @@
         <v>3.98</v>
       </c>
     </row>
-    <row r="206" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A206" s="29" t="s">
         <v>282</v>
       </c>
@@ -28362,7 +28362,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="207" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A207" s="29" t="s">
         <v>283</v>
       </c>
@@ -28483,7 +28483,7 @@
         <v>8.3333333333333331E-5</v>
       </c>
     </row>
-    <row r="208" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A208" s="90" t="s">
         <v>361</v>
       </c>
@@ -28604,7 +28604,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="209" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A209" s="2" t="s">
         <v>608</v>
       </c>
@@ -28752,7 +28752,7 @@
         <v>21.36</v>
       </c>
     </row>
-    <row r="210" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A210" s="2" t="s">
         <v>618</v>
       </c>
@@ -28873,7 +28873,7 @@
         <v>-30000</v>
       </c>
     </row>
-    <row r="211" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A211" s="2" t="s">
         <v>513</v>
       </c>
@@ -28994,7 +28994,7 @@
         <v>-100000</v>
       </c>
     </row>
-    <row r="212" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A212" s="2" t="s">
         <v>609</v>
       </c>
@@ -29135,7 +29135,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="213" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A213" s="2" t="s">
         <v>505</v>
       </c>
@@ -29256,7 +29256,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="214" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A214" s="2" t="s">
         <v>506</v>
       </c>
@@ -29377,7 +29377,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="215" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A215" s="2" t="s">
         <v>507</v>
       </c>
@@ -29498,7 +29498,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="216" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A216" s="2" t="s">
         <v>515</v>
       </c>
@@ -29619,7 +29619,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="217" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A217" s="2" t="s">
         <v>517</v>
       </c>
@@ -29773,7 +29773,7 @@
         <v>2.5000000000000001E-4</v>
       </c>
     </row>
-    <row r="218" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A218" s="2" t="s">
         <v>522</v>
       </c>
@@ -29894,7 +29894,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="219" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A219" s="2" t="s">
         <v>550</v>
       </c>
@@ -30015,7 +30015,7 @@
         <v>2.4999999999999999E-13</v>
       </c>
     </row>
-    <row r="220" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A220" s="2" t="s">
         <v>553</v>
       </c>
@@ -30156,7 +30156,7 @@
         <v>1.1999999999999999E-7</v>
       </c>
     </row>
-    <row r="221" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A221" s="2" t="s">
         <v>570</v>
       </c>
@@ -30277,7 +30277,7 @@
         <v>1E-8</v>
       </c>
     </row>
-    <row r="222" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A222" s="2" t="s">
         <v>555</v>
       </c>
@@ -30400,7 +30400,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="223" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A223" s="2" t="s">
         <v>520</v>
       </c>
@@ -30429,132 +30429,132 @@
       </c>
       <c r="I223" s="98"/>
       <c r="J223" s="98">
-        <f t="shared" ref="J223:AO223" si="24">0.00000000000001*10000*8</f>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" ref="J223:K223" si="24">0.00000000000001*100000</f>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="K223" s="98">
         <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="L223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f>0.00000000000001*100000</f>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="M223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" ref="M223:AC223" si="25">0.00000000000001*100000</f>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="N223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="O223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="P223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="Q223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="R223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="S223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="T223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="U223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="V223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="W223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="X223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="Y223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="Z223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="AA223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="AB223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="AC223" s="98">
-        <f t="shared" si="24"/>
-        <v>8.0000000000000003E-10</v>
+        <f t="shared" si="25"/>
+        <v>1.0000000000000001E-9</v>
       </c>
       <c r="AD223" s="98"/>
       <c r="AE223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" ref="J223:AO223" si="26">0.00000000000001*10000*8</f>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AF223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AG223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AH223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AI223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AJ223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AK223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AL223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AM223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AN223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
       <c r="AO223" s="98">
-        <f t="shared" si="24"/>
+        <f t="shared" si="26"/>
         <v>8.0000000000000003E-10</v>
       </c>
     </row>
-    <row r="224" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A224" s="2" t="s">
         <v>564</v>
       </c>
@@ -30583,132 +30583,132 @@
       </c>
       <c r="I224" s="98"/>
       <c r="J224" s="98">
-        <f t="shared" ref="J224:K224" si="25">J223*10</f>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" ref="J224:K224" si="27">J223*10</f>
+        <v>1E-8</v>
       </c>
       <c r="K224" s="98">
-        <f t="shared" si="25"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="27"/>
+        <v>1E-8</v>
       </c>
       <c r="L224" s="98">
-        <f t="shared" ref="L224:N224" si="26">L223*10</f>
-        <v>8.0000000000000005E-9</v>
+        <f>L223*10</f>
+        <v>1E-8</v>
       </c>
       <c r="M224" s="98">
-        <f t="shared" si="26"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" ref="L224:N224" si="28">M223*10</f>
+        <v>1E-8</v>
       </c>
       <c r="N224" s="98">
-        <f t="shared" si="26"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="28"/>
+        <v>1E-8</v>
       </c>
       <c r="O224" s="98">
-        <f t="shared" ref="O224:R224" si="27">O223*10</f>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" ref="O224:R224" si="29">O223*10</f>
+        <v>1E-8</v>
       </c>
       <c r="P224" s="98">
-        <f t="shared" si="27"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="29"/>
+        <v>1E-8</v>
       </c>
       <c r="Q224" s="98">
-        <f t="shared" si="27"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="29"/>
+        <v>1E-8</v>
       </c>
       <c r="R224" s="98">
-        <f t="shared" si="27"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="29"/>
+        <v>1E-8</v>
       </c>
       <c r="S224" s="98">
-        <f t="shared" ref="S224:V224" si="28">S223*10</f>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" ref="S224:V224" si="30">S223*10</f>
+        <v>1E-8</v>
       </c>
       <c r="T224" s="98">
-        <f t="shared" si="28"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="30"/>
+        <v>1E-8</v>
       </c>
       <c r="U224" s="98">
-        <f t="shared" si="28"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="30"/>
+        <v>1E-8</v>
       </c>
       <c r="V224" s="98">
-        <f t="shared" si="28"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="30"/>
+        <v>1E-8</v>
       </c>
       <c r="W224" s="98">
-        <f t="shared" ref="W224:AA224" si="29">W223*10</f>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" ref="W224:AA224" si="31">W223*10</f>
+        <v>1E-8</v>
       </c>
       <c r="X224" s="98">
-        <f t="shared" si="29"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="31"/>
+        <v>1E-8</v>
       </c>
       <c r="Y224" s="98">
-        <f t="shared" si="29"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="31"/>
+        <v>1E-8</v>
       </c>
       <c r="Z224" s="98">
-        <f t="shared" si="29"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="31"/>
+        <v>1E-8</v>
       </c>
       <c r="AA224" s="98">
-        <f t="shared" si="29"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="31"/>
+        <v>1E-8</v>
       </c>
       <c r="AB224" s="98">
-        <f t="shared" ref="AB224:AC224" si="30">AB223*10</f>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" ref="AB224:AC224" si="32">AB223*10</f>
+        <v>1E-8</v>
       </c>
       <c r="AC224" s="98">
-        <f t="shared" si="30"/>
-        <v>8.0000000000000005E-9</v>
+        <f t="shared" si="32"/>
+        <v>1E-8</v>
       </c>
       <c r="AD224" s="98"/>
       <c r="AE224" s="98">
-        <f t="shared" ref="AE224:AO224" si="31">AE223*10</f>
+        <f t="shared" ref="AE224:AO224" si="33">AE223*10</f>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AF224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AG224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AH224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AI224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AJ224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AK224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AL224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AM224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AN224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
       <c r="AO224" s="98">
-        <f t="shared" si="31"/>
+        <f t="shared" si="33"/>
         <v>8.0000000000000005E-9</v>
       </c>
     </row>
-    <row r="225" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A225" s="2" t="s">
         <v>566</v>
       </c>
@@ -30737,101 +30737,132 @@
       </c>
       <c r="I225" s="98"/>
       <c r="J225" s="98">
-        <v>10</v>
+        <f t="shared" ref="J225:AC225" si="34">0.84*(0.36^2)</f>
+        <v>0.10886399999999999</v>
       </c>
       <c r="K225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="L225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="M225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="N225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="O225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="P225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="Q225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="R225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="S225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="T225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="U225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="V225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="W225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="X225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="Y225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="Z225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AA225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AB225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AC225" s="98">
-        <v>10</v>
+        <f t="shared" si="34"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AD225" s="98"/>
       <c r="AE225" s="98">
-        <v>10</v>
+        <f t="shared" ref="AE225:AO225" si="35">0.84*(0.36^2)</f>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AF225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AG225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AH225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AI225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AJ225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AK225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AL225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AM225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AN225" s="98">
-        <v>10</v>
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
       </c>
       <c r="AO225" s="98">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="226" spans="1:41" x14ac:dyDescent="0.25">
+        <f t="shared" si="35"/>
+        <v>0.10886399999999999</v>
+      </c>
+    </row>
+    <row r="226" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A226" s="2" t="s">
         <v>610</v>
       </c>
@@ -30952,7 +30983,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="227" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A227" s="2" t="s">
         <v>611</v>
       </c>
@@ -31073,7 +31104,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="228" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A228" s="2" t="s">
         <v>612</v>
       </c>
@@ -31102,11 +31133,11 @@
       </c>
       <c r="I228" s="99"/>
       <c r="J228" s="99">
-        <f t="shared" ref="J228:K228" si="32">2*0.075</f>
+        <f t="shared" ref="J228:K228" si="36">2*0.075</f>
         <v>0.15</v>
       </c>
       <c r="K228" s="99">
-        <f t="shared" si="32"/>
+        <f t="shared" si="36"/>
         <v>0.15</v>
       </c>
       <c r="L228" s="99">
@@ -31114,120 +31145,120 @@
         <v>0.15</v>
       </c>
       <c r="M228" s="99">
-        <f t="shared" ref="M228:AC228" si="33">2*0.075</f>
+        <f t="shared" ref="M228:AC228" si="37">2*0.075</f>
         <v>0.15</v>
       </c>
       <c r="N228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="O228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="P228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="Q228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="R228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="S228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="T228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="U228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="V228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="W228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="X228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="Y228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="Z228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="AA228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="AB228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="AC228" s="99">
-        <f t="shared" si="33"/>
+        <f t="shared" si="37"/>
         <v>0.15</v>
       </c>
       <c r="AD228" s="99"/>
       <c r="AE228" s="99">
-        <f t="shared" ref="AE228:AO228" si="34">2*0.1</f>
+        <f t="shared" ref="AE228:AO228" si="38">2*0.1</f>
         <v>0.2</v>
       </c>
       <c r="AF228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AG228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AH228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AI228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AJ228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AK228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AL228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AM228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AN228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
       <c r="AO228" s="99">
-        <f t="shared" si="34"/>
+        <f t="shared" si="38"/>
         <v>0.2</v>
       </c>
     </row>
-    <row r="229" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A229" s="2" t="s">
         <v>613</v>
       </c>
@@ -31348,7 +31379,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="230" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A230" s="2" t="s">
         <v>619</v>
       </c>
@@ -31374,127 +31405,127 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="J230" s="97">
-        <f t="shared" ref="J230:AC230" si="35">0.00001*10</f>
+        <f t="shared" ref="J230:AC230" si="39">0.00001*10</f>
         <v>1E-4</v>
       </c>
       <c r="K230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="L230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="M230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="N230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="O230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="P230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="Q230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="R230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="S230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="T230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="U230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="V230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="W230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="X230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="Y230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="Z230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="AA230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="AB230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="AC230" s="97">
-        <f t="shared" si="35"/>
+        <f t="shared" si="39"/>
         <v>1E-4</v>
       </c>
       <c r="AE230" s="97">
-        <f t="shared" ref="AE230:AO230" si="36">0.00001</f>
+        <f t="shared" ref="AE230:AO230" si="40">0.00001</f>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AF230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AG230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AH230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AI230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AJ230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AK230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AL230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AM230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AN230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="AO230" s="97">
-        <f t="shared" si="36"/>
+        <f t="shared" si="40"/>
         <v>1.0000000000000001E-5</v>
       </c>
     </row>
@@ -31764,13 +31795,13 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="49.5703125" customWidth="1"/>
+    <col min="1" max="2" width="35.6640625" customWidth="1"/>
+    <col min="3" max="3" width="49.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>285</v>
       </c>
@@ -31781,7 +31812,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>205</v>
       </c>
@@ -31793,7 +31824,7 @@
         <v>pi</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -31805,7 +31836,7 @@
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>39</v>
       </c>
@@ -31817,7 +31848,7 @@
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>206</v>
       </c>
@@ -31829,7 +31860,7 @@
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>41</v>
       </c>
@@ -31841,7 +31872,7 @@
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>40</v>
       </c>
@@ -31853,7 +31884,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>44</v>
       </c>
@@ -31865,7 +31896,7 @@
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>49</v>
       </c>
@@ -31877,7 +31908,7 @@
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>47</v>
       </c>
@@ -31889,7 +31920,7 @@
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>48</v>
       </c>
@@ -31901,7 +31932,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>46</v>
       </c>
@@ -31913,7 +31944,7 @@
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -31925,7 +31956,7 @@
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>90</v>
       </c>
@@ -31937,7 +31968,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -31949,7 +31980,7 @@
         <v/>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>207</v>
       </c>
@@ -31961,7 +31992,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>43</v>
       </c>
@@ -31973,7 +32004,7 @@
         <v/>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -31985,7 +32016,7 @@
         <v/>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>204</v>
       </c>
@@ -31997,7 +32028,7 @@
         <v/>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>51</v>
       </c>
@@ -32009,7 +32040,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>52</v>
       </c>
@@ -32021,7 +32052,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>53</v>
       </c>
@@ -32033,7 +32064,7 @@
         <v/>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -32045,7 +32076,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>54</v>
       </c>
@@ -32057,7 +32088,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>60</v>
       </c>
@@ -32069,7 +32100,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>208</v>
       </c>
@@ -32081,7 +32112,7 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>209</v>
       </c>
@@ -32093,7 +32124,7 @@
         <v>root_growth_T_ref</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>210</v>
       </c>
@@ -32105,7 +32136,7 @@
         <v>root_growth_A</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>211</v>
       </c>
@@ -32117,7 +32148,7 @@
         <v>root_growth_B</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>212</v>
       </c>
@@ -32129,7 +32160,7 @@
         <v>root_growth_C</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>213</v>
       </c>
@@ -32141,7 +32172,7 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>214</v>
       </c>
@@ -32153,7 +32184,7 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>215</v>
       </c>
@@ -32165,7 +32196,7 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>216</v>
       </c>
@@ -32177,7 +32208,7 @@
         <v/>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>217</v>
       </c>
@@ -32189,7 +32220,7 @@
         <v/>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>61</v>
       </c>
@@ -32201,7 +32232,7 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>75</v>
       </c>
@@ -32213,7 +32244,7 @@
         <v/>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>218</v>
       </c>
@@ -32225,7 +32256,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>219</v>
       </c>
@@ -32237,7 +32268,7 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>220</v>
       </c>
@@ -32249,7 +32280,7 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>221</v>
       </c>
@@ -32261,7 +32292,7 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>76</v>
       </c>
@@ -32273,7 +32304,7 @@
         <v/>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>222</v>
       </c>
@@ -32285,7 +32316,7 @@
         <v>expected_C_sucrose_root</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>223</v>
       </c>
@@ -32297,7 +32328,7 @@
         <v>expected_C_hexose_root</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>224</v>
       </c>
@@ -32309,7 +32340,7 @@
         <v>expected_C_hexose_soil</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>225</v>
       </c>
@@ -32321,7 +32352,7 @@
         <v>expected_C_hexose_reserve</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>65</v>
       </c>
@@ -32333,7 +32364,7 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>77</v>
       </c>
@@ -32345,7 +32376,7 @@
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>226</v>
       </c>
@@ -32357,7 +32388,7 @@
         <v>surfacic_unloading_rate_reference</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>227</v>
       </c>
@@ -32369,7 +32400,7 @@
         <v>surfacic_unloading_rate_primordium</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>66</v>
       </c>
@@ -32381,7 +32412,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>228</v>
       </c>
@@ -32393,7 +32424,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>229</v>
       </c>
@@ -32405,7 +32436,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>230</v>
       </c>
@@ -32417,7 +32448,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>231</v>
       </c>
@@ -32429,7 +32460,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>68</v>
       </c>
@@ -32441,7 +32472,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>232</v>
       </c>
@@ -32453,7 +32484,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>233</v>
       </c>
@@ -32465,7 +32496,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>234</v>
       </c>
@@ -32477,7 +32508,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>235</v>
       </c>
@@ -32489,7 +32520,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>67</v>
       </c>
@@ -32501,7 +32532,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>70</v>
       </c>
@@ -32513,7 +32544,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>69</v>
       </c>
@@ -32525,7 +32556,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>57</v>
       </c>
@@ -32537,7 +32568,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>56</v>
       </c>
@@ -32549,7 +32580,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>58</v>
       </c>
@@ -32561,7 +32592,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>71</v>
       </c>
@@ -32573,7 +32604,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>236</v>
       </c>
@@ -32585,7 +32616,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>237</v>
       </c>
@@ -32597,7 +32628,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>238</v>
       </c>
@@ -32609,7 +32640,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>239</v>
       </c>
@@ -32621,7 +32652,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -32633,7 +32664,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -32645,7 +32676,7 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>240</v>
       </c>
@@ -32657,7 +32688,7 @@
         <v/>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>241</v>
       </c>
@@ -32669,7 +32700,7 @@
         <v/>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>242</v>
       </c>
@@ -32681,7 +32712,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>243</v>
       </c>
@@ -32693,7 +32724,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -32705,7 +32736,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>244</v>
       </c>
@@ -32717,7 +32748,7 @@
         <v>expected_exudation_efflux</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>78</v>
       </c>
@@ -32729,7 +32760,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>245</v>
       </c>
@@ -32741,7 +32772,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>246</v>
       </c>
@@ -32753,7 +32784,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>247</v>
       </c>
@@ -32765,7 +32796,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>248</v>
       </c>
@@ -32777,7 +32808,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>79</v>
       </c>
@@ -32789,7 +32820,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>80</v>
       </c>
@@ -32801,7 +32832,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>249</v>
       </c>
@@ -32813,7 +32844,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>250</v>
       </c>
@@ -32825,7 +32856,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>251</v>
       </c>
@@ -32837,7 +32868,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>252</v>
       </c>
@@ -32849,7 +32880,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>81</v>
       </c>
@@ -32861,7 +32892,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>253</v>
       </c>
@@ -32873,7 +32904,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>254</v>
       </c>
@@ -32885,7 +32916,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>255</v>
       </c>
@@ -32897,7 +32928,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>256</v>
       </c>
@@ -32909,7 +32940,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>257</v>
       </c>
@@ -32921,7 +32952,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>258</v>
       </c>
@@ -32933,7 +32964,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>259</v>
       </c>
@@ -32945,7 +32976,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>260</v>
       </c>
@@ -32957,7 +32988,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>261</v>
       </c>
@@ -32969,7 +33000,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>262</v>
       </c>
@@ -32981,7 +33012,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>263</v>
       </c>
@@ -32993,7 +33024,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>264</v>
       </c>
@@ -33005,7 +33036,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>265</v>
       </c>
@@ -33017,7 +33048,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>266</v>
       </c>
@@ -33029,7 +33060,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>267</v>
       </c>
@@ -33041,7 +33072,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>268</v>
       </c>
@@ -33053,7 +33084,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>269</v>
       </c>
@@ -33065,7 +33096,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>270</v>
       </c>
@@ -33077,7 +33108,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>271</v>
       </c>
@@ -33089,7 +33120,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>272</v>
       </c>
@@ -33101,7 +33132,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>273</v>
       </c>
@@ -33113,7 +33144,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>274</v>
       </c>
@@ -33125,7 +33156,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>275</v>
       </c>
@@ -33137,7 +33168,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>276</v>
       </c>
@@ -33149,7 +33180,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>277</v>
       </c>
@@ -33161,7 +33192,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>278</v>
       </c>
@@ -33173,7 +33204,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>279</v>
       </c>
@@ -33185,7 +33216,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>280</v>
       </c>
@@ -33197,7 +33228,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>281</v>
       </c>
@@ -33209,7 +33240,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>282</v>
       </c>
@@ -33221,7 +33252,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>283</v>
       </c>
@@ -33233,7 +33264,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>59</v>
       </c>
@@ -33245,7 +33276,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>62</v>
       </c>
@@ -33257,7 +33288,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>64</v>
       </c>
@@ -33269,7 +33300,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>63</v>
       </c>
@@ -33281,7 +33312,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>82</v>
       </c>
@@ -33293,7 +33324,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>83</v>
       </c>
@@ -33305,7 +33336,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>85</v>
       </c>
@@ -33317,7 +33348,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>84</v>
       </c>
@@ -33329,7 +33360,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>2</v>
       </c>
@@ -33341,7 +33372,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>4</v>
       </c>
@@ -33353,7 +33384,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>5</v>
       </c>
@@ -33365,7 +33396,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>20</v>
       </c>
@@ -33377,7 +33408,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>0</v>
       </c>
@@ -33389,7 +33420,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>1</v>
       </c>
@@ -33401,7 +33432,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>6</v>
       </c>
@@ -33413,7 +33444,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>7</v>
       </c>
@@ -33425,7 +33456,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>8</v>
       </c>
@@ -33437,7 +33468,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>9</v>
       </c>
@@ -33449,7 +33480,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>10</v>
       </c>
@@ -33461,7 +33492,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>11</v>
       </c>
@@ -33473,7 +33504,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>12</v>
       </c>
@@ -33485,7 +33516,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>13</v>
       </c>
@@ -33497,7 +33528,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>14</v>
       </c>
@@ -33509,7 +33540,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>15</v>
       </c>
@@ -33521,7 +33552,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>16</v>
       </c>
@@ -33533,7 +33564,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>17</v>
       </c>
@@ -33545,7 +33576,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>18</v>
       </c>
@@ -33557,7 +33588,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>19</v>
       </c>
@@ -33569,7 +33600,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>21</v>
       </c>
@@ -33581,7 +33612,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>22</v>
       </c>
@@ -33593,7 +33624,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>23</v>
       </c>
@@ -33605,7 +33636,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>24</v>
       </c>
@@ -33617,7 +33648,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>25</v>
       </c>
@@ -33629,7 +33660,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>26</v>
       </c>
@@ -33641,7 +33672,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>27</v>
       </c>
@@ -33653,7 +33684,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>28</v>
       </c>
@@ -33662,7 +33693,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>29</v>
       </c>
@@ -33671,7 +33702,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>30</v>
       </c>
@@ -33680,7 +33711,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>31</v>
       </c>
@@ -33689,7 +33720,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>32</v>
       </c>
@@ -33698,7 +33729,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>33</v>
       </c>
@@ -33707,7 +33738,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>34</v>
       </c>
@@ -33716,7 +33747,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>35</v>
       </c>
@@ -33725,7 +33756,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>36</v>
       </c>
@@ -33734,7 +33765,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>37</v>
       </c>
@@ -33743,7 +33774,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>38</v>
       </c>
@@ -33752,7 +33783,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>361</v>
       </c>

</xml_diff>